<commit_message>
Small changes in expected values. Mostly added min(100,x) in cases.
</commit_message>
<xml_diff>
--- a/specifications/3_MechRemove/ScriptRules_MechRemove.xlsx
+++ b/specifications/3_MechRemove/ScriptRules_MechRemove.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11025" windowHeight="9615" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11025" windowHeight="9615" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="FBDescriptions" sheetId="9" r:id="rId1"/>
@@ -2591,8 +2591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K951"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B60" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="K102" sqref="K102"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7596,8 +7596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94:A1048576"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8031,7 +8031,7 @@
         <v>100</v>
       </c>
       <c r="K5" s="12">
-        <f t="shared" ref="K5" si="8">J5</f>
+        <f t="shared" ref="K5:K15" si="8">J5</f>
         <v>0</v>
       </c>
       <c r="L5" s="15">
@@ -8043,7 +8043,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="12">
-        <f t="shared" ref="O5" si="10">N5</f>
+        <f t="shared" ref="O5:O15" si="10">N5</f>
         <v>0</v>
       </c>
       <c r="P5" s="15">
@@ -8058,7 +8058,7 @@
         <v>25</v>
       </c>
       <c r="S5" s="12">
-        <f t="shared" ref="S5" si="12">R5</f>
+        <f t="shared" ref="S5:S15" si="12">R5</f>
         <v>25</v>
       </c>
       <c r="T5" s="15">
@@ -8073,7 +8073,7 @@
         <v>60</v>
       </c>
       <c r="W5" s="12">
-        <f t="shared" ref="W5" si="14">V5</f>
+        <f t="shared" ref="W5:W15" si="14">V5</f>
         <v>60</v>
       </c>
       <c r="X5" s="15">
@@ -8088,7 +8088,7 @@
         <v>78</v>
       </c>
       <c r="AA5" s="12">
-        <f t="shared" ref="AA5" si="16">Z5</f>
+        <f t="shared" ref="AA5:AA15" si="16">Z5</f>
         <v>78</v>
       </c>
       <c r="AB5" s="15">
@@ -8498,7 +8498,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="12">
-        <f t="shared" ref="K10" si="18">J10</f>
+        <f t="shared" ref="K10:K20" si="18">J10</f>
         <v>0</v>
       </c>
       <c r="L10" s="15">
@@ -8510,7 +8510,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="12">
-        <f t="shared" ref="O10" si="19">N10</f>
+        <f t="shared" ref="O10:O20" si="19">N10</f>
         <v>0</v>
       </c>
       <c r="P10" s="15">
@@ -8522,7 +8522,7 @@
         <v>0</v>
       </c>
       <c r="S10" s="12">
-        <f t="shared" ref="S10" si="20">R10</f>
+        <f t="shared" ref="S10:S20" si="20">R10</f>
         <v>0</v>
       </c>
       <c r="T10" s="15">
@@ -8537,7 +8537,7 @@
         <v>44</v>
       </c>
       <c r="W10" s="12">
-        <f t="shared" ref="W10" si="21">V10</f>
+        <f t="shared" ref="W10:W20" si="21">V10</f>
         <v>44</v>
       </c>
       <c r="X10" s="15">
@@ -8549,7 +8549,7 @@
         <v>44</v>
       </c>
       <c r="AA10" s="12">
-        <f t="shared" ref="AA10" si="22">Z10</f>
+        <f t="shared" ref="AA10:AA20" si="22">Z10</f>
         <v>0</v>
       </c>
       <c r="AB10" s="15">
@@ -8763,7 +8763,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="12">
-        <f t="shared" ref="K13:K15" si="23">J13</f>
+        <f t="shared" ref="K13:K23" si="23">J13</f>
         <v>0</v>
       </c>
       <c r="L13" s="15">
@@ -8775,7 +8775,7 @@
         <v>0</v>
       </c>
       <c r="O13" s="12">
-        <f t="shared" ref="O13:O15" si="24">N13</f>
+        <f t="shared" ref="O13:O23" si="24">N13</f>
         <v>0</v>
       </c>
       <c r="P13" s="15">
@@ -8790,7 +8790,7 @@
         <v>0.5</v>
       </c>
       <c r="S13" s="12">
-        <f t="shared" ref="S13:S15" si="25">R13</f>
+        <f t="shared" ref="S13:S23" si="25">R13</f>
         <v>0.5</v>
       </c>
       <c r="T13" s="15">
@@ -8805,7 +8805,7 @@
         <v>1.7</v>
       </c>
       <c r="W13" s="12">
-        <f t="shared" ref="W13:W15" si="26">V13</f>
+        <f t="shared" ref="W13:W23" si="26">V13</f>
         <v>1.7</v>
       </c>
       <c r="X13" s="15">
@@ -8820,7 +8820,7 @@
         <v>1</v>
       </c>
       <c r="AA13" s="12">
-        <f t="shared" ref="AA13:AA15" si="27">Z13</f>
+        <f t="shared" ref="AA13:AA23" si="27">Z13</f>
         <v>1</v>
       </c>
       <c r="AB13" s="15">
@@ -10698,7 +10698,7 @@
         <v>5</v>
       </c>
       <c r="M34" s="16">
-        <f t="shared" ref="M34" si="42">L34</f>
+        <f t="shared" ref="M34:M44" si="42">L34</f>
         <v>5</v>
       </c>
       <c r="N34" s="11">
@@ -10713,7 +10713,7 @@
         <v>3</v>
       </c>
       <c r="Q34" s="16">
-        <f t="shared" ref="Q34" si="43">P34</f>
+        <f t="shared" ref="Q34:Q44" si="43">P34</f>
         <v>3</v>
       </c>
       <c r="R34" s="11">
@@ -10728,7 +10728,7 @@
         <v>5</v>
       </c>
       <c r="U34" s="16">
-        <f t="shared" ref="U34" si="44">T34</f>
+        <f t="shared" ref="U34:U44" si="44">T34</f>
         <v>5</v>
       </c>
       <c r="V34" s="11">
@@ -10743,7 +10743,7 @@
         <v>6</v>
       </c>
       <c r="Y34" s="16">
-        <f t="shared" ref="Y34" si="45">X34</f>
+        <f t="shared" ref="Y34:Y44" si="45">X34</f>
         <v>6</v>
       </c>
       <c r="Z34" s="11">
@@ -10758,7 +10758,7 @@
         <v>5</v>
       </c>
       <c r="AC34" s="16">
-        <f t="shared" ref="AC34" si="46">AB34</f>
+        <f t="shared" ref="AC34:AC44" si="46">AB34</f>
         <v>5</v>
       </c>
     </row>
@@ -11008,66 +11008,66 @@
         <v>2</v>
       </c>
       <c r="K37" s="12">
-        <f t="shared" ref="K37" si="49">J37</f>
+        <f t="shared" ref="K37:K44" si="49">J37</f>
         <v>2</v>
       </c>
       <c r="L37" s="15">
-        <f t="shared" ref="L37" si="50">K37</f>
+        <f t="shared" ref="L37:L44" si="50">K37</f>
         <v>2</v>
       </c>
       <c r="M37" s="16">
-        <f t="shared" ref="M37" si="51">L37</f>
+        <f t="shared" ref="M37:M47" si="51">L37</f>
         <v>2</v>
       </c>
       <c r="O37" s="12">
-        <f t="shared" ref="O37" si="52">N37</f>
+        <f t="shared" ref="O37:O44" si="52">N37</f>
         <v>0</v>
       </c>
       <c r="P37" s="15">
-        <f t="shared" ref="P37" si="53">O37</f>
+        <f t="shared" ref="P37:P44" si="53">O37</f>
         <v>0</v>
       </c>
       <c r="Q37" s="16">
-        <f t="shared" ref="Q37" si="54">P37</f>
+        <f t="shared" ref="Q37:Q47" si="54">P37</f>
         <v>0</v>
       </c>
       <c r="R37" s="11">
         <v>1</v>
       </c>
       <c r="S37" s="12">
-        <f t="shared" ref="S37" si="55">R37</f>
+        <f t="shared" ref="S37:S44" si="55">R37</f>
         <v>1</v>
       </c>
       <c r="T37" s="15">
-        <f t="shared" ref="T37" si="56">S37</f>
+        <f t="shared" ref="T37:T44" si="56">S37</f>
         <v>1</v>
       </c>
       <c r="U37" s="16">
-        <f t="shared" ref="U37" si="57">T37</f>
+        <f t="shared" ref="U37:U47" si="57">T37</f>
         <v>1</v>
       </c>
       <c r="W37" s="12">
-        <f t="shared" ref="W37" si="58">V37</f>
+        <f t="shared" ref="W37:W44" si="58">V37</f>
         <v>0</v>
       </c>
       <c r="X37" s="15">
-        <f t="shared" ref="X37" si="59">W37</f>
+        <f t="shared" ref="X37:X44" si="59">W37</f>
         <v>0</v>
       </c>
       <c r="Y37" s="16">
-        <f t="shared" ref="Y37" si="60">X37</f>
+        <f t="shared" ref="Y37:Y47" si="60">X37</f>
         <v>0</v>
       </c>
       <c r="AA37" s="12">
-        <f t="shared" ref="AA37" si="61">Z37</f>
+        <f t="shared" ref="AA37:AA44" si="61">Z37</f>
         <v>0</v>
       </c>
       <c r="AB37" s="15">
-        <f t="shared" ref="AB37" si="62">AA37</f>
+        <f t="shared" ref="AB37:AB44" si="62">AA37</f>
         <v>0</v>
       </c>
       <c r="AC37" s="16">
-        <f t="shared" ref="AC37" si="63">AB37</f>
+        <f t="shared" ref="AC37:AC47" si="63">AB37</f>
         <v>0</v>
       </c>
     </row>
@@ -11214,7 +11214,7 @@
         <v>85</v>
       </c>
       <c r="M39" s="16">
-        <f t="shared" ref="M39:M40" si="64">L39</f>
+        <f t="shared" ref="M39:M49" si="64">L39</f>
         <v>85</v>
       </c>
       <c r="O39" s="12">
@@ -11226,7 +11226,7 @@
         <v>0</v>
       </c>
       <c r="Q39" s="16">
-        <f t="shared" ref="Q39:Q40" si="65">P39</f>
+        <f t="shared" ref="Q39:Q49" si="65">P39</f>
         <v>0</v>
       </c>
       <c r="R39" s="11">
@@ -11241,7 +11241,7 @@
         <v>90</v>
       </c>
       <c r="U39" s="16">
-        <f t="shared" ref="U39:U40" si="66">T39</f>
+        <f t="shared" ref="U39:U49" si="66">T39</f>
         <v>90</v>
       </c>
       <c r="W39" s="12">
@@ -11253,7 +11253,7 @@
         <v>0</v>
       </c>
       <c r="Y39" s="16">
-        <f t="shared" ref="Y39:Y40" si="67">X39</f>
+        <f t="shared" ref="Y39:Y49" si="67">X39</f>
         <v>0</v>
       </c>
       <c r="AA39" s="12">
@@ -11265,7 +11265,7 @@
         <v>0</v>
       </c>
       <c r="AC39" s="16">
-        <f t="shared" ref="AC39:AC40" si="68">AB39</f>
+        <f t="shared" ref="AC39:AC49" si="68">AB39</f>
         <v>0</v>
       </c>
     </row>
@@ -11296,11 +11296,11 @@
         <v>0.9</v>
       </c>
       <c r="K40" s="12">
-        <f t="shared" ref="K40" si="69">J40</f>
+        <f t="shared" ref="K40:K47" si="69">J40</f>
         <v>0</v>
       </c>
       <c r="L40" s="15">
-        <f t="shared" ref="L40" si="70">K40</f>
+        <f t="shared" ref="L40:L47" si="70">K40</f>
         <v>0</v>
       </c>
       <c r="M40" s="16">
@@ -11311,11 +11311,11 @@
         <v>2</v>
       </c>
       <c r="O40" s="12">
-        <f t="shared" ref="O40" si="71">N40</f>
+        <f t="shared" ref="O40:O47" si="71">N40</f>
         <v>2</v>
       </c>
       <c r="P40" s="15">
-        <f t="shared" ref="P40" si="72">O40</f>
+        <f t="shared" ref="P40:P47" si="72">O40</f>
         <v>2</v>
       </c>
       <c r="Q40" s="16">
@@ -11326,11 +11326,11 @@
         <v>1</v>
       </c>
       <c r="S40" s="12">
-        <f t="shared" ref="S40" si="73">R40</f>
+        <f t="shared" ref="S40:S47" si="73">R40</f>
         <v>1</v>
       </c>
       <c r="T40" s="15">
-        <f t="shared" ref="T40" si="74">S40</f>
+        <f t="shared" ref="T40:T47" si="74">S40</f>
         <v>1</v>
       </c>
       <c r="U40" s="16">
@@ -11341,11 +11341,11 @@
         <v>2.5</v>
       </c>
       <c r="W40" s="12">
-        <f t="shared" ref="W40" si="75">V40</f>
+        <f t="shared" ref="W40:W47" si="75">V40</f>
         <v>2.5</v>
       </c>
       <c r="X40" s="15">
-        <f t="shared" ref="X40" si="76">W40</f>
+        <f t="shared" ref="X40:X47" si="76">W40</f>
         <v>2.5</v>
       </c>
       <c r="Y40" s="16">
@@ -11356,11 +11356,11 @@
         <v>2</v>
       </c>
       <c r="AA40" s="12">
-        <f t="shared" ref="AA40" si="77">Z40</f>
+        <f t="shared" ref="AA40:AA47" si="77">Z40</f>
         <v>2</v>
       </c>
       <c r="AB40" s="15">
-        <f t="shared" ref="AB40" si="78">AA40</f>
+        <f t="shared" ref="AB40:AB47" si="78">AA40</f>
         <v>2</v>
       </c>
       <c r="AC40" s="16">
@@ -11620,7 +11620,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="16">
-        <f t="shared" ref="M43:M44" si="79">L43</f>
+        <f t="shared" ref="M43:M53" si="79">L43</f>
         <v>0</v>
       </c>
       <c r="N43" s="11">
@@ -11635,7 +11635,7 @@
         <v>85</v>
       </c>
       <c r="Q43" s="16">
-        <f t="shared" ref="Q43:Q44" si="80">P43</f>
+        <f t="shared" ref="Q43:Q53" si="80">P43</f>
         <v>85</v>
       </c>
       <c r="R43" s="11">
@@ -11650,7 +11650,7 @@
         <v>90</v>
       </c>
       <c r="U43" s="16">
-        <f t="shared" ref="U43:U44" si="81">T43</f>
+        <f t="shared" ref="U43:U53" si="81">T43</f>
         <v>90</v>
       </c>
       <c r="V43" s="11">
@@ -11665,7 +11665,7 @@
         <v>80</v>
       </c>
       <c r="Y43" s="16">
-        <f t="shared" ref="Y43:Y44" si="82">X43</f>
+        <f t="shared" ref="Y43:Y53" si="82">X43</f>
         <v>80</v>
       </c>
       <c r="Z43" s="11">
@@ -11680,7 +11680,7 @@
         <v>60</v>
       </c>
       <c r="AC43" s="16">
-        <f t="shared" ref="AC43:AC44" si="83">AB43</f>
+        <f t="shared" ref="AC43:AC53" si="83">AB43</f>
         <v>60</v>
       </c>
     </row>
@@ -11711,11 +11711,11 @@
         <v>0.9</v>
       </c>
       <c r="K44" s="12">
-        <f t="shared" ref="K44" si="84">J44</f>
+        <f t="shared" ref="K44:K51" si="84">J44</f>
         <v>0</v>
       </c>
       <c r="L44" s="15">
-        <f t="shared" ref="L44" si="85">K44</f>
+        <f t="shared" ref="L44:L51" si="85">K44</f>
         <v>0</v>
       </c>
       <c r="M44" s="16">
@@ -11726,11 +11726,11 @@
         <v>1</v>
       </c>
       <c r="O44" s="12">
-        <f t="shared" ref="O44" si="86">N44</f>
+        <f t="shared" ref="O44:O51" si="86">N44</f>
         <v>1</v>
       </c>
       <c r="P44" s="15">
-        <f t="shared" ref="P44" si="87">O44</f>
+        <f t="shared" ref="P44:P51" si="87">O44</f>
         <v>1</v>
       </c>
       <c r="Q44" s="16">
@@ -11741,11 +11741,11 @@
         <v>0.5</v>
       </c>
       <c r="S44" s="12">
-        <f t="shared" ref="S44" si="88">R44</f>
+        <f t="shared" ref="S44:S51" si="88">R44</f>
         <v>0.5</v>
       </c>
       <c r="T44" s="15">
-        <f t="shared" ref="T44" si="89">S44</f>
+        <f t="shared" ref="T44:T51" si="89">S44</f>
         <v>0.5</v>
       </c>
       <c r="U44" s="16">
@@ -11753,11 +11753,11 @@
         <v>0.5</v>
       </c>
       <c r="W44" s="12">
-        <f t="shared" ref="W44" si="90">V44</f>
+        <f t="shared" ref="W44:W51" si="90">V44</f>
         <v>0</v>
       </c>
       <c r="X44" s="15">
-        <f t="shared" ref="X44" si="91">W44</f>
+        <f t="shared" ref="X44:X51" si="91">W44</f>
         <v>0</v>
       </c>
       <c r="Y44" s="16">
@@ -11768,11 +11768,11 @@
         <v>1</v>
       </c>
       <c r="AA44" s="12">
-        <f t="shared" ref="AA44" si="92">Z44</f>
+        <f t="shared" ref="AA44:AA51" si="92">Z44</f>
         <v>1</v>
       </c>
       <c r="AB44" s="15">
-        <f t="shared" ref="AB44" si="93">AA44</f>
+        <f t="shared" ref="AB44:AB51" si="93">AA44</f>
         <v>1</v>
       </c>
       <c r="AC44" s="16">
@@ -12126,7 +12126,7 @@
         <v>0.75</v>
       </c>
       <c r="L48" s="15">
-        <f t="shared" ref="L48:L52" si="98">K48</f>
+        <f t="shared" ref="L48:L77" si="98">K48</f>
         <v>0.75</v>
       </c>
       <c r="M48" s="16">
@@ -12138,7 +12138,7 @@
         <v>0</v>
       </c>
       <c r="P48" s="15">
-        <f t="shared" ref="P48:P52" si="101">O48</f>
+        <f t="shared" ref="P48:P77" si="101">O48</f>
         <v>0</v>
       </c>
       <c r="Q48" s="16">
@@ -12153,7 +12153,7 @@
         <v>0.375</v>
       </c>
       <c r="T48" s="15">
-        <f t="shared" ref="T48:T52" si="104">S48</f>
+        <f t="shared" ref="T48:T77" si="104">S48</f>
         <v>0.375</v>
       </c>
       <c r="U48" s="16">
@@ -12168,7 +12168,7 @@
         <v>0.75</v>
       </c>
       <c r="X48" s="15">
-        <f t="shared" ref="X48:X52" si="107">W48</f>
+        <f t="shared" ref="X48:X77" si="107">W48</f>
         <v>0.75</v>
       </c>
       <c r="Y48" s="16">
@@ -12183,7 +12183,7 @@
         <v>0.375</v>
       </c>
       <c r="AB48" s="15">
-        <f t="shared" ref="AB48:AB52" si="110">AA48</f>
+        <f t="shared" ref="AB48:AB77" si="110">AA48</f>
         <v>0.375</v>
       </c>
       <c r="AC48" s="16">
@@ -13248,11 +13248,11 @@
         <v>0</v>
       </c>
       <c r="K59" s="12">
-        <f t="shared" ref="K59:K60" si="113">J59</f>
+        <f t="shared" ref="K59:K93" si="113">J59</f>
         <v>0</v>
       </c>
       <c r="L59" s="15">
-        <f t="shared" ref="L59:L79" si="114">K59</f>
+        <f t="shared" ref="L59:L88" si="114">K59</f>
         <v>0</v>
       </c>
       <c r="M59" s="16">
@@ -13260,11 +13260,11 @@
         <v>0</v>
       </c>
       <c r="O59" s="12">
-        <f t="shared" ref="O59:O60" si="115">N59</f>
+        <f t="shared" ref="O59:O93" si="115">N59</f>
         <v>0</v>
       </c>
       <c r="P59" s="15">
-        <f t="shared" ref="P59:P79" si="116">O59</f>
+        <f t="shared" ref="P59:P88" si="116">O59</f>
         <v>0</v>
       </c>
       <c r="Q59" s="16">
@@ -13275,11 +13275,11 @@
         <v>3.5</v>
       </c>
       <c r="S59" s="12">
-        <f t="shared" ref="S59:S60" si="117">R59</f>
+        <f t="shared" ref="S59:S93" si="117">R59</f>
         <v>3.5</v>
       </c>
       <c r="T59" s="15">
-        <f t="shared" ref="T59:T79" si="118">S59</f>
+        <f t="shared" ref="T59:T88" si="118">S59</f>
         <v>3.5</v>
       </c>
       <c r="U59" s="16">
@@ -13287,11 +13287,11 @@
         <v>0</v>
       </c>
       <c r="W59" s="12">
-        <f t="shared" ref="W59:W60" si="119">V59</f>
+        <f t="shared" ref="W59:W93" si="119">V59</f>
         <v>0</v>
       </c>
       <c r="X59" s="15">
-        <f t="shared" ref="X59:X79" si="120">W59</f>
+        <f t="shared" ref="X59:X88" si="120">W59</f>
         <v>0</v>
       </c>
       <c r="Y59" s="16">
@@ -13299,11 +13299,11 @@
         <v>0</v>
       </c>
       <c r="AA59" s="12">
-        <f t="shared" ref="AA59:AA60" si="121">Z59</f>
+        <f t="shared" ref="AA59:AA93" si="121">Z59</f>
         <v>0</v>
       </c>
       <c r="AB59" s="15">
-        <f t="shared" ref="AB59:AB79" si="122">AA59</f>
+        <f t="shared" ref="AB59:AB88" si="122">AA59</f>
         <v>0</v>
       </c>
       <c r="AC59" s="16">
@@ -13524,7 +13524,7 @@
         <v>9.6</v>
       </c>
       <c r="K62" s="12">
-        <f t="shared" ref="K62:K67" si="123">J62</f>
+        <f t="shared" ref="K62:K93" si="123">J62</f>
         <v>0</v>
       </c>
       <c r="L62" s="15">
@@ -13536,7 +13536,7 @@
         <v>0</v>
       </c>
       <c r="O62" s="12">
-        <f t="shared" ref="O62:O67" si="124">N62</f>
+        <f t="shared" ref="O62:O93" si="124">N62</f>
         <v>0</v>
       </c>
       <c r="P62" s="15">
@@ -13551,7 +13551,7 @@
         <v>3.5</v>
       </c>
       <c r="S62" s="12">
-        <f t="shared" ref="S62:S67" si="125">R62</f>
+        <f t="shared" ref="S62:S93" si="125">R62</f>
         <v>3.5</v>
       </c>
       <c r="T62" s="15">
@@ -13566,7 +13566,7 @@
         <v>10</v>
       </c>
       <c r="W62" s="12">
-        <f t="shared" ref="W62:W67" si="126">V62</f>
+        <f t="shared" ref="W62:W93" si="126">V62</f>
         <v>10</v>
       </c>
       <c r="X62" s="15">
@@ -13581,7 +13581,7 @@
         <v>10</v>
       </c>
       <c r="AA62" s="12">
-        <f t="shared" ref="AA62:AA67" si="127">Z62</f>
+        <f t="shared" ref="AA62:AA93" si="127">Z62</f>
         <v>10</v>
       </c>
       <c r="AB62" s="15">
@@ -14287,7 +14287,7 @@
         <v>0</v>
       </c>
       <c r="M70" s="16">
-        <f t="shared" ref="M70:M77" si="129">L70</f>
+        <f t="shared" ref="M70:M93" si="129">L70</f>
         <v>0</v>
       </c>
       <c r="N70" s="11">
@@ -14302,7 +14302,7 @@
         <v>0</v>
       </c>
       <c r="Q70" s="16">
-        <f t="shared" ref="Q70:Q77" si="130">P70</f>
+        <f t="shared" ref="Q70:Q93" si="130">P70</f>
         <v>0</v>
       </c>
       <c r="R70" s="11">
@@ -14317,7 +14317,7 @@
         <v>0</v>
       </c>
       <c r="U70" s="16">
-        <f t="shared" ref="U70:U77" si="131">T70</f>
+        <f t="shared" ref="U70:U93" si="131">T70</f>
         <v>0</v>
       </c>
       <c r="V70" s="11">
@@ -14332,7 +14332,7 @@
         <v>0</v>
       </c>
       <c r="Y70" s="16">
-        <f t="shared" ref="Y70:Y77" si="132">X70</f>
+        <f t="shared" ref="Y70:Y93" si="132">X70</f>
         <v>0</v>
       </c>
       <c r="Z70" s="11">
@@ -14347,7 +14347,7 @@
         <v>0</v>
       </c>
       <c r="AC70" s="16">
-        <f t="shared" ref="AC70:AC77" si="133">AB70</f>
+        <f t="shared" ref="AC70:AC93" si="133">AB70</f>
         <v>0</v>
       </c>
     </row>
@@ -14375,7 +14375,7 @@
         <v>0</v>
       </c>
       <c r="K71" s="12">
-        <f t="shared" ref="K71:K77" si="134">J71</f>
+        <f t="shared" ref="K71:K93" si="134">J71</f>
         <v>0</v>
       </c>
       <c r="L71" s="15">
@@ -14387,7 +14387,7 @@
         <v>0</v>
       </c>
       <c r="O71" s="12">
-        <f t="shared" ref="O71:O77" si="135">N71</f>
+        <f t="shared" ref="O71:O93" si="135">N71</f>
         <v>0</v>
       </c>
       <c r="P71" s="15">
@@ -14399,7 +14399,7 @@
         <v>0</v>
       </c>
       <c r="S71" s="12">
-        <f t="shared" ref="S71:S77" si="136">R71</f>
+        <f t="shared" ref="S71:S93" si="136">R71</f>
         <v>0</v>
       </c>
       <c r="T71" s="15">
@@ -14414,7 +14414,7 @@
         <v>90</v>
       </c>
       <c r="W71" s="12">
-        <f t="shared" ref="W71:W77" si="137">V71</f>
+        <f t="shared" ref="W71:W93" si="137">V71</f>
         <v>90</v>
       </c>
       <c r="X71" s="15">
@@ -14426,7 +14426,7 @@
         <v>90</v>
       </c>
       <c r="AA71" s="12">
-        <f t="shared" ref="AA71:AA77" si="138">Z71</f>
+        <f t="shared" ref="AA71:AA93" si="138">Z71</f>
         <v>0</v>
       </c>
       <c r="AB71" s="15">
@@ -14995,7 +14995,7 @@
         <v>0</v>
       </c>
       <c r="K78" s="12">
-        <f t="shared" ref="K78:K89" si="140">$C78*J78</f>
+        <f t="shared" ref="K78:K92" si="140">$C78*J78</f>
         <v>0</v>
       </c>
       <c r="L78" s="15">
@@ -15007,7 +15007,7 @@
         <v>0</v>
       </c>
       <c r="O78" s="12">
-        <f t="shared" ref="O78:O89" si="141">$C78*N78</f>
+        <f t="shared" ref="O78:O92" si="141">$C78*N78</f>
         <v>0</v>
       </c>
       <c r="P78" s="15">
@@ -15022,7 +15022,7 @@
         <v>2</v>
       </c>
       <c r="S78" s="12">
-        <f t="shared" ref="S78:S89" si="142">$C78*R78</f>
+        <f t="shared" ref="S78:S92" si="142">$C78*R78</f>
         <v>1.5</v>
       </c>
       <c r="T78" s="15">
@@ -15034,7 +15034,7 @@
         <v>2</v>
       </c>
       <c r="W78" s="12">
-        <f t="shared" ref="W78:W89" si="143">$C78*V78</f>
+        <f t="shared" ref="W78:W92" si="143">$C78*V78</f>
         <v>0</v>
       </c>
       <c r="X78" s="15">
@@ -15046,7 +15046,7 @@
         <v>0</v>
       </c>
       <c r="AA78" s="12">
-        <f t="shared" ref="AA78:AA89" si="144">$C78*Z78</f>
+        <f t="shared" ref="AA78:AA92" si="144">$C78*Z78</f>
         <v>0</v>
       </c>
       <c r="AB78" s="15">
@@ -15083,7 +15083,7 @@
         <v>0</v>
       </c>
       <c r="I79" s="16">
-        <f>$E79*H79</f>
+        <f>MIN(100,$E79*H79)</f>
         <v>0</v>
       </c>
       <c r="K79" s="12">
@@ -15095,7 +15095,7 @@
         <v>0</v>
       </c>
       <c r="M79" s="16">
-        <f>$E79*L79</f>
+        <f>MIN(100,$E79*L79)</f>
         <v>0</v>
       </c>
       <c r="O79" s="12">
@@ -15107,7 +15107,7 @@
         <v>0</v>
       </c>
       <c r="Q79" s="16">
-        <f>$E79*P79</f>
+        <f>MIN(100,$E79*P79)</f>
         <v>0</v>
       </c>
       <c r="R79" s="11">
@@ -15122,7 +15122,7 @@
         <v>3.75</v>
       </c>
       <c r="U79" s="16">
-        <f>$E79*T79</f>
+        <f>MIN(100,$E79*T79)</f>
         <v>5</v>
       </c>
       <c r="W79" s="12">
@@ -15134,7 +15134,7 @@
         <v>0</v>
       </c>
       <c r="Y79" s="16">
-        <f>$E79*X79</f>
+        <f>MIN(100,$E79*X79)</f>
         <v>0</v>
       </c>
       <c r="AA79" s="12">
@@ -15146,7 +15146,7 @@
         <v>0</v>
       </c>
       <c r="AC79" s="16">
-        <f>$E79*AB79</f>
+        <f>MIN(100,$E79*AB79)</f>
         <v>0</v>
       </c>
     </row>
@@ -15281,7 +15281,7 @@
         <v>52.5</v>
       </c>
       <c r="H81" s="15">
-        <f t="shared" si="145"/>
+        <f>MIN(100,G81*$D81)</f>
         <v>70</v>
       </c>
       <c r="I81" s="16">
@@ -15296,11 +15296,11 @@
         <v>45</v>
       </c>
       <c r="L81" s="15">
-        <f t="shared" si="146"/>
+        <f>MIN(100,K81*$D81)</f>
         <v>60</v>
       </c>
       <c r="M81" s="16">
-        <f t="shared" ref="M81" si="151">L81</f>
+        <f t="shared" ref="M81:M93" si="151">L81</f>
         <v>60</v>
       </c>
       <c r="N81" s="11">
@@ -15311,11 +15311,11 @@
         <v>3.75</v>
       </c>
       <c r="P81" s="15">
-        <f t="shared" si="147"/>
+        <f>MIN(100,O81*$D81)</f>
         <v>5</v>
       </c>
       <c r="Q81" s="16">
-        <f t="shared" ref="Q81" si="152">P81</f>
+        <f t="shared" ref="Q81:Q93" si="152">P81</f>
         <v>5</v>
       </c>
       <c r="R81" s="11">
@@ -15326,11 +15326,11 @@
         <v>11.25</v>
       </c>
       <c r="T81" s="15">
-        <f t="shared" si="148"/>
+        <f>MIN(100,S81*$D81)</f>
         <v>15</v>
       </c>
       <c r="U81" s="16">
-        <f t="shared" ref="U81" si="153">T81</f>
+        <f t="shared" ref="U81:U93" si="153">T81</f>
         <v>15</v>
       </c>
       <c r="V81" s="11">
@@ -15341,11 +15341,11 @@
         <v>67.5</v>
       </c>
       <c r="X81" s="15">
-        <f t="shared" si="149"/>
+        <f>MIN(100,W81*$D81)</f>
         <v>90</v>
       </c>
       <c r="Y81" s="16">
-        <f t="shared" ref="Y81" si="154">X81</f>
+        <f t="shared" ref="Y81:Y93" si="154">X81</f>
         <v>90</v>
       </c>
       <c r="Z81" s="11">
@@ -15356,11 +15356,11 @@
         <v>52.5</v>
       </c>
       <c r="AB81" s="15">
-        <f t="shared" si="150"/>
+        <f>MIN(100,AA81*$D81)</f>
         <v>70</v>
       </c>
       <c r="AC81" s="16">
-        <f t="shared" ref="AC81" si="155">AB81</f>
+        <f t="shared" ref="AC81:AC93" si="155">AB81</f>
         <v>70</v>
       </c>
     </row>
@@ -15484,7 +15484,7 @@
         <v>0</v>
       </c>
       <c r="I83" s="16">
-        <f>$E83*H83</f>
+        <f>MIN(100,$E83*H83)</f>
         <v>0</v>
       </c>
       <c r="K83" s="12">
@@ -15496,7 +15496,7 @@
         <v>0</v>
       </c>
       <c r="M83" s="16">
-        <f>$E83*L83</f>
+        <f>MIN(100,$E83*L83)</f>
         <v>0</v>
       </c>
       <c r="O83" s="12">
@@ -15508,7 +15508,7 @@
         <v>0</v>
       </c>
       <c r="Q83" s="16">
-        <f>$E83*P83</f>
+        <f>MIN(100,$E83*P83)</f>
         <v>0</v>
       </c>
       <c r="R83" s="11">
@@ -15523,7 +15523,7 @@
         <v>60</v>
       </c>
       <c r="U83" s="16">
-        <f>$E83*T83</f>
+        <f>MIN(100,$E83*T83)</f>
         <v>80</v>
       </c>
       <c r="V83" s="11">
@@ -15538,7 +15538,7 @@
         <v>3.75</v>
       </c>
       <c r="Y83" s="16">
-        <f>$E83*X83</f>
+        <f>MIN(100,$E83*X83)</f>
         <v>5</v>
       </c>
       <c r="AA83" s="12">
@@ -15550,7 +15550,7 @@
         <v>0</v>
       </c>
       <c r="AC83" s="16">
-        <f>$E83*AB83</f>
+        <f>MIN(100,$E83*AB83)</f>
         <v>0</v>
       </c>
     </row>
@@ -16142,7 +16142,7 @@
         <v>0</v>
       </c>
       <c r="K90" s="12">
-        <f t="shared" ref="K90" si="166">J90</f>
+        <f t="shared" ref="K90:K93" si="166">J90</f>
         <v>0</v>
       </c>
       <c r="L90" s="15">
@@ -16154,7 +16154,7 @@
         <v>0</v>
       </c>
       <c r="O90" s="12">
-        <f t="shared" ref="O90" si="167">N90</f>
+        <f t="shared" ref="O90:O93" si="167">N90</f>
         <v>0</v>
       </c>
       <c r="P90" s="15">
@@ -16166,7 +16166,7 @@
         <v>0</v>
       </c>
       <c r="S90" s="12">
-        <f t="shared" ref="S90" si="168">R90</f>
+        <f t="shared" ref="S90:S93" si="168">R90</f>
         <v>0</v>
       </c>
       <c r="T90" s="15">
@@ -16178,7 +16178,7 @@
         <v>0</v>
       </c>
       <c r="W90" s="12">
-        <f t="shared" ref="W90" si="169">V90</f>
+        <f t="shared" ref="W90:W93" si="169">V90</f>
         <v>0</v>
       </c>
       <c r="X90" s="15">
@@ -16190,7 +16190,7 @@
         <v>0</v>
       </c>
       <c r="AA90" s="12">
-        <f t="shared" ref="AA90" si="170">Z90</f>
+        <f t="shared" ref="AA90:AA93" si="170">Z90</f>
         <v>0</v>
       </c>
       <c r="AB90" s="15">
@@ -16317,7 +16317,7 @@
         <v>0</v>
       </c>
       <c r="K92" s="12">
-        <f t="shared" ref="K92" si="171">$C92*J92</f>
+        <f t="shared" ref="K92:K93" si="171">$C92*J92</f>
         <v>0</v>
       </c>
       <c r="L92" s="15">
@@ -16329,7 +16329,7 @@
         <v>0</v>
       </c>
       <c r="O92" s="12">
-        <f t="shared" ref="O92" si="172">$C92*N92</f>
+        <f t="shared" ref="O92:O93" si="172">$C92*N92</f>
         <v>0</v>
       </c>
       <c r="P92" s="15">
@@ -16344,7 +16344,7 @@
         <v>1</v>
       </c>
       <c r="S92" s="12">
-        <f t="shared" ref="S92" si="173">$C92*R92</f>
+        <f t="shared" ref="S92:S93" si="173">$C92*R92</f>
         <v>0.75</v>
       </c>
       <c r="T92" s="15">
@@ -16356,7 +16356,7 @@
         <v>0.75</v>
       </c>
       <c r="W92" s="12">
-        <f t="shared" ref="W92" si="174">$C92*V92</f>
+        <f t="shared" ref="W92:W93" si="174">$C92*V92</f>
         <v>0</v>
       </c>
       <c r="X92" s="15">
@@ -16368,7 +16368,7 @@
         <v>0</v>
       </c>
       <c r="AA92" s="12">
-        <f t="shared" ref="AA92" si="175">$C92*Z92</f>
+        <f t="shared" ref="AA92:AA93" si="175">$C92*Z92</f>
         <v>0</v>
       </c>
       <c r="AB92" s="15">
@@ -16477,8 +16477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94:A1048576"/>
+    <sheetView topLeftCell="L1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16913,7 +16913,7 @@
         <v>100</v>
       </c>
       <c r="K5" s="12">
-        <f t="shared" ref="K5" si="7">J5</f>
+        <f t="shared" ref="K5:K20" si="7">J5</f>
         <v>0</v>
       </c>
       <c r="L5" s="15">
@@ -16925,7 +16925,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="12">
-        <f t="shared" ref="O5" si="9">N5</f>
+        <f t="shared" ref="O5:O20" si="9">N5</f>
         <v>0</v>
       </c>
       <c r="P5" s="15">
@@ -16940,7 +16940,7 @@
         <v>25</v>
       </c>
       <c r="S5" s="12">
-        <f t="shared" ref="S5" si="11">R5</f>
+        <f t="shared" ref="S5:S20" si="11">R5</f>
         <v>25</v>
       </c>
       <c r="T5" s="15">
@@ -16955,7 +16955,7 @@
         <v>60</v>
       </c>
       <c r="W5" s="12">
-        <f t="shared" ref="W5" si="13">V5</f>
+        <f t="shared" ref="W5:W20" si="13">V5</f>
         <v>60</v>
       </c>
       <c r="X5" s="15">
@@ -16970,7 +16970,7 @@
         <v>78</v>
       </c>
       <c r="AA5" s="12">
-        <f t="shared" ref="AA5" si="15">Z5</f>
+        <f t="shared" ref="AA5:AA20" si="15">Z5</f>
         <v>78</v>
       </c>
       <c r="AB5" s="15">
@@ -17380,7 +17380,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="12">
-        <f t="shared" ref="K10" si="17">J10</f>
+        <f t="shared" ref="K10:K25" si="17">J10</f>
         <v>0</v>
       </c>
       <c r="L10" s="15">
@@ -17392,7 +17392,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="12">
-        <f t="shared" ref="O10" si="18">N10</f>
+        <f t="shared" ref="O10:O25" si="18">N10</f>
         <v>0</v>
       </c>
       <c r="P10" s="15">
@@ -17404,7 +17404,7 @@
         <v>0</v>
       </c>
       <c r="S10" s="12">
-        <f t="shared" ref="S10" si="19">R10</f>
+        <f t="shared" ref="S10:S25" si="19">R10</f>
         <v>0</v>
       </c>
       <c r="T10" s="15">
@@ -17419,7 +17419,7 @@
         <v>44</v>
       </c>
       <c r="W10" s="12">
-        <f t="shared" ref="W10" si="20">V10</f>
+        <f t="shared" ref="W10:W25" si="20">V10</f>
         <v>44</v>
       </c>
       <c r="X10" s="15">
@@ -17431,7 +17431,7 @@
         <v>44</v>
       </c>
       <c r="AA10" s="12">
-        <f t="shared" ref="AA10" si="21">Z10</f>
+        <f t="shared" ref="AA10:AA25" si="21">Z10</f>
         <v>0</v>
       </c>
       <c r="AB10" s="15">
@@ -19586,7 +19586,7 @@
         <v>5</v>
       </c>
       <c r="M34" s="16">
-        <f t="shared" ref="M34" si="41">L34</f>
+        <f t="shared" ref="M34:M47" si="41">L34</f>
         <v>5</v>
       </c>
       <c r="N34" s="11">
@@ -19601,7 +19601,7 @@
         <v>3</v>
       </c>
       <c r="Q34" s="16">
-        <f t="shared" ref="Q34" si="42">P34</f>
+        <f t="shared" ref="Q34:Q47" si="42">P34</f>
         <v>3</v>
       </c>
       <c r="R34" s="11">
@@ -19616,7 +19616,7 @@
         <v>5</v>
       </c>
       <c r="U34" s="16">
-        <f t="shared" ref="U34" si="43">T34</f>
+        <f t="shared" ref="U34:U47" si="43">T34</f>
         <v>5</v>
       </c>
       <c r="V34" s="11">
@@ -19631,7 +19631,7 @@
         <v>6</v>
       </c>
       <c r="Y34" s="16">
-        <f t="shared" ref="Y34" si="44">X34</f>
+        <f t="shared" ref="Y34:Y47" si="44">X34</f>
         <v>6</v>
       </c>
       <c r="Z34" s="11">
@@ -19646,7 +19646,7 @@
         <v>5</v>
       </c>
       <c r="AC34" s="16">
-        <f t="shared" ref="AC34" si="45">AB34</f>
+        <f t="shared" ref="AC34:AC47" si="45">AB34</f>
         <v>5</v>
       </c>
     </row>
@@ -19896,66 +19896,66 @@
         <v>2</v>
       </c>
       <c r="K37" s="12">
-        <f t="shared" ref="K37" si="47">J37</f>
+        <f t="shared" ref="K37:K44" si="47">J37</f>
         <v>2</v>
       </c>
       <c r="L37" s="15">
-        <f t="shared" ref="L37" si="48">K37</f>
+        <f t="shared" ref="L37:L44" si="48">K37</f>
         <v>2</v>
       </c>
       <c r="M37" s="16">
-        <f t="shared" ref="M37" si="49">L37</f>
+        <f t="shared" ref="M37:M50" si="49">L37</f>
         <v>2</v>
       </c>
       <c r="O37" s="12">
-        <f t="shared" ref="O37" si="50">N37</f>
+        <f t="shared" ref="O37:O44" si="50">N37</f>
         <v>0</v>
       </c>
       <c r="P37" s="15">
-        <f t="shared" ref="P37" si="51">O37</f>
+        <f t="shared" ref="P37:P44" si="51">O37</f>
         <v>0</v>
       </c>
       <c r="Q37" s="16">
-        <f t="shared" ref="Q37" si="52">P37</f>
+        <f t="shared" ref="Q37:Q50" si="52">P37</f>
         <v>0</v>
       </c>
       <c r="R37" s="11">
         <v>1</v>
       </c>
       <c r="S37" s="12">
-        <f t="shared" ref="S37" si="53">R37</f>
+        <f t="shared" ref="S37:S44" si="53">R37</f>
         <v>1</v>
       </c>
       <c r="T37" s="15">
-        <f t="shared" ref="T37" si="54">S37</f>
+        <f t="shared" ref="T37:T44" si="54">S37</f>
         <v>1</v>
       </c>
       <c r="U37" s="16">
-        <f t="shared" ref="U37" si="55">T37</f>
+        <f t="shared" ref="U37:U50" si="55">T37</f>
         <v>1</v>
       </c>
       <c r="W37" s="12">
-        <f t="shared" ref="W37" si="56">V37</f>
+        <f t="shared" ref="W37:W44" si="56">V37</f>
         <v>0</v>
       </c>
       <c r="X37" s="15">
-        <f t="shared" ref="X37" si="57">W37</f>
+        <f t="shared" ref="X37:X44" si="57">W37</f>
         <v>0</v>
       </c>
       <c r="Y37" s="16">
-        <f t="shared" ref="Y37" si="58">X37</f>
+        <f t="shared" ref="Y37:Y50" si="58">X37</f>
         <v>0</v>
       </c>
       <c r="AA37" s="12">
-        <f t="shared" ref="AA37" si="59">Z37</f>
+        <f t="shared" ref="AA37:AA44" si="59">Z37</f>
         <v>0</v>
       </c>
       <c r="AB37" s="15">
-        <f t="shared" ref="AB37" si="60">AA37</f>
+        <f t="shared" ref="AB37:AB44" si="60">AA37</f>
         <v>0</v>
       </c>
       <c r="AC37" s="16">
-        <f t="shared" ref="AC37" si="61">AB37</f>
+        <f t="shared" ref="AC37:AC50" si="61">AB37</f>
         <v>0</v>
       </c>
     </row>
@@ -20102,7 +20102,7 @@
         <v>85</v>
       </c>
       <c r="M39" s="16">
-        <f t="shared" ref="M39:M40" si="62">L39</f>
+        <f t="shared" ref="M39:M52" si="62">L39</f>
         <v>85</v>
       </c>
       <c r="O39" s="12">
@@ -20114,7 +20114,7 @@
         <v>0</v>
       </c>
       <c r="Q39" s="16">
-        <f t="shared" ref="Q39:Q40" si="63">P39</f>
+        <f t="shared" ref="Q39:Q52" si="63">P39</f>
         <v>0</v>
       </c>
       <c r="R39" s="11">
@@ -20129,7 +20129,7 @@
         <v>90</v>
       </c>
       <c r="U39" s="16">
-        <f t="shared" ref="U39:U40" si="64">T39</f>
+        <f t="shared" ref="U39:U52" si="64">T39</f>
         <v>90</v>
       </c>
       <c r="W39" s="12">
@@ -20141,7 +20141,7 @@
         <v>0</v>
       </c>
       <c r="Y39" s="16">
-        <f t="shared" ref="Y39:Y40" si="65">X39</f>
+        <f t="shared" ref="Y39:Y52" si="65">X39</f>
         <v>0</v>
       </c>
       <c r="AA39" s="12">
@@ -20153,7 +20153,7 @@
         <v>0</v>
       </c>
       <c r="AC39" s="16">
-        <f t="shared" ref="AC39:AC40" si="66">AB39</f>
+        <f t="shared" ref="AC39:AC52" si="66">AB39</f>
         <v>0</v>
       </c>
     </row>
@@ -20184,11 +20184,11 @@
         <v>0.9</v>
       </c>
       <c r="K40" s="12">
-        <f t="shared" ref="K40" si="67">J40</f>
+        <f t="shared" ref="K40:K47" si="67">J40</f>
         <v>0</v>
       </c>
       <c r="L40" s="15">
-        <f t="shared" ref="L40" si="68">K40</f>
+        <f t="shared" ref="L40:L47" si="68">K40</f>
         <v>0</v>
       </c>
       <c r="M40" s="16">
@@ -20199,11 +20199,11 @@
         <v>2</v>
       </c>
       <c r="O40" s="12">
-        <f t="shared" ref="O40" si="69">N40</f>
+        <f t="shared" ref="O40:O47" si="69">N40</f>
         <v>2</v>
       </c>
       <c r="P40" s="15">
-        <f t="shared" ref="P40" si="70">O40</f>
+        <f t="shared" ref="P40:P47" si="70">O40</f>
         <v>2</v>
       </c>
       <c r="Q40" s="16">
@@ -20214,11 +20214,11 @@
         <v>1</v>
       </c>
       <c r="S40" s="12">
-        <f t="shared" ref="S40" si="71">R40</f>
+        <f t="shared" ref="S40:S47" si="71">R40</f>
         <v>1</v>
       </c>
       <c r="T40" s="15">
-        <f t="shared" ref="T40" si="72">S40</f>
+        <f t="shared" ref="T40:T47" si="72">S40</f>
         <v>1</v>
       </c>
       <c r="U40" s="16">
@@ -20229,11 +20229,11 @@
         <v>2.5</v>
       </c>
       <c r="W40" s="12">
-        <f t="shared" ref="W40" si="73">V40</f>
+        <f t="shared" ref="W40:W47" si="73">V40</f>
         <v>2.5</v>
       </c>
       <c r="X40" s="15">
-        <f t="shared" ref="X40" si="74">W40</f>
+        <f t="shared" ref="X40:X47" si="74">W40</f>
         <v>2.5</v>
       </c>
       <c r="Y40" s="16">
@@ -20244,11 +20244,11 @@
         <v>2</v>
       </c>
       <c r="AA40" s="12">
-        <f t="shared" ref="AA40" si="75">Z40</f>
+        <f t="shared" ref="AA40:AA47" si="75">Z40</f>
         <v>2</v>
       </c>
       <c r="AB40" s="15">
-        <f t="shared" ref="AB40" si="76">AA40</f>
+        <f t="shared" ref="AB40:AB47" si="76">AA40</f>
         <v>2</v>
       </c>
       <c r="AC40" s="16">
@@ -20508,7 +20508,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="16">
-        <f t="shared" ref="M43:M44" si="77">L43</f>
+        <f t="shared" ref="M43:M56" si="77">L43</f>
         <v>0</v>
       </c>
       <c r="N43" s="11">
@@ -20523,7 +20523,7 @@
         <v>85</v>
       </c>
       <c r="Q43" s="16">
-        <f t="shared" ref="Q43:Q44" si="78">P43</f>
+        <f t="shared" ref="Q43:Q56" si="78">P43</f>
         <v>85</v>
       </c>
       <c r="R43" s="11">
@@ -20538,7 +20538,7 @@
         <v>90</v>
       </c>
       <c r="U43" s="16">
-        <f t="shared" ref="U43:U44" si="79">T43</f>
+        <f t="shared" ref="U43:U56" si="79">T43</f>
         <v>90</v>
       </c>
       <c r="V43" s="11">
@@ -20553,7 +20553,7 @@
         <v>80</v>
       </c>
       <c r="Y43" s="16">
-        <f t="shared" ref="Y43:Y44" si="80">X43</f>
+        <f t="shared" ref="Y43:Y56" si="80">X43</f>
         <v>80</v>
       </c>
       <c r="Z43" s="11">
@@ -20568,7 +20568,7 @@
         <v>60</v>
       </c>
       <c r="AC43" s="16">
-        <f t="shared" ref="AC43:AC44" si="81">AB43</f>
+        <f t="shared" ref="AC43:AC56" si="81">AB43</f>
         <v>60</v>
       </c>
     </row>
@@ -20599,11 +20599,11 @@
         <v>0.9</v>
       </c>
       <c r="K44" s="12">
-        <f t="shared" ref="K44" si="82">J44</f>
+        <f t="shared" ref="K44:K51" si="82">J44</f>
         <v>0</v>
       </c>
       <c r="L44" s="15">
-        <f t="shared" ref="L44" si="83">K44</f>
+        <f t="shared" ref="L44:L51" si="83">K44</f>
         <v>0</v>
       </c>
       <c r="M44" s="16">
@@ -20614,11 +20614,11 @@
         <v>1</v>
       </c>
       <c r="O44" s="12">
-        <f t="shared" ref="O44" si="84">N44</f>
+        <f t="shared" ref="O44:O51" si="84">N44</f>
         <v>1</v>
       </c>
       <c r="P44" s="15">
-        <f t="shared" ref="P44" si="85">O44</f>
+        <f t="shared" ref="P44:P51" si="85">O44</f>
         <v>1</v>
       </c>
       <c r="Q44" s="16">
@@ -20629,11 +20629,11 @@
         <v>0.5</v>
       </c>
       <c r="S44" s="12">
-        <f t="shared" ref="S44" si="86">R44</f>
+        <f t="shared" ref="S44:S51" si="86">R44</f>
         <v>0.5</v>
       </c>
       <c r="T44" s="15">
-        <f t="shared" ref="T44" si="87">S44</f>
+        <f t="shared" ref="T44:T51" si="87">S44</f>
         <v>0.5</v>
       </c>
       <c r="U44" s="16">
@@ -20641,11 +20641,11 @@
         <v>0.5</v>
       </c>
       <c r="W44" s="12">
-        <f t="shared" ref="W44" si="88">V44</f>
+        <f t="shared" ref="W44:W51" si="88">V44</f>
         <v>0</v>
       </c>
       <c r="X44" s="15">
-        <f t="shared" ref="X44" si="89">W44</f>
+        <f t="shared" ref="X44:X51" si="89">W44</f>
         <v>0</v>
       </c>
       <c r="Y44" s="16">
@@ -20656,11 +20656,11 @@
         <v>1</v>
       </c>
       <c r="AA44" s="12">
-        <f t="shared" ref="AA44" si="90">Z44</f>
+        <f t="shared" ref="AA44:AA51" si="90">Z44</f>
         <v>1</v>
       </c>
       <c r="AB44" s="15">
-        <f t="shared" ref="AB44" si="91">AA44</f>
+        <f t="shared" ref="AB44:AB51" si="91">AA44</f>
         <v>1</v>
       </c>
       <c r="AC44" s="16">
@@ -20914,7 +20914,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="16">
-        <f t="shared" ref="M47" si="92">L47</f>
+        <f t="shared" ref="M47:M60" si="92">L47</f>
         <v>0</v>
       </c>
       <c r="N47" s="11">
@@ -20929,7 +20929,7 @@
         <v>70</v>
       </c>
       <c r="Q47" s="16">
-        <f t="shared" ref="Q47" si="93">P47</f>
+        <f t="shared" ref="Q47:Q60" si="93">P47</f>
         <v>70</v>
       </c>
       <c r="R47" s="11">
@@ -20944,7 +20944,7 @@
         <v>90</v>
       </c>
       <c r="U47" s="16">
-        <f t="shared" ref="U47" si="94">T47</f>
+        <f t="shared" ref="U47:U60" si="94">T47</f>
         <v>90</v>
       </c>
       <c r="W47" s="12">
@@ -20956,7 +20956,7 @@
         <v>0</v>
       </c>
       <c r="Y47" s="16">
-        <f t="shared" ref="Y47" si="95">X47</f>
+        <f t="shared" ref="Y47:Y60" si="95">X47</f>
         <v>0</v>
       </c>
       <c r="Z47" s="11">
@@ -20971,7 +20971,7 @@
         <v>60</v>
       </c>
       <c r="AC47" s="16">
-        <f t="shared" ref="AC47" si="96">AB47</f>
+        <f t="shared" ref="AC47:AC60" si="96">AB47</f>
         <v>60</v>
       </c>
     </row>
@@ -21014,7 +21014,7 @@
         <v>0.5</v>
       </c>
       <c r="L48" s="15">
-        <f t="shared" ref="L48:L52" si="99">K48</f>
+        <f t="shared" ref="L48:L77" si="99">K48</f>
         <v>0.5</v>
       </c>
       <c r="M48" s="16">
@@ -21026,7 +21026,7 @@
         <v>0</v>
       </c>
       <c r="P48" s="15">
-        <f t="shared" ref="P48:P52" si="101">O48</f>
+        <f t="shared" ref="P48:P77" si="101">O48</f>
         <v>0</v>
       </c>
       <c r="Q48" s="16">
@@ -21041,7 +21041,7 @@
         <v>0.25</v>
       </c>
       <c r="T48" s="15">
-        <f t="shared" ref="T48:T52" si="103">S48</f>
+        <f t="shared" ref="T48:T77" si="103">S48</f>
         <v>0.25</v>
       </c>
       <c r="U48" s="16">
@@ -21056,7 +21056,7 @@
         <v>0.5</v>
       </c>
       <c r="X48" s="15">
-        <f t="shared" ref="X48:X52" si="105">W48</f>
+        <f t="shared" ref="X48:X77" si="105">W48</f>
         <v>0.5</v>
       </c>
       <c r="Y48" s="16">
@@ -21071,7 +21071,7 @@
         <v>0.25</v>
       </c>
       <c r="AB48" s="15">
-        <f t="shared" ref="AB48:AB52" si="107">AA48</f>
+        <f t="shared" ref="AB48:AB77" si="107">AA48</f>
         <v>0.25</v>
       </c>
       <c r="AC48" s="16">
@@ -22136,11 +22136,11 @@
         <v>0</v>
       </c>
       <c r="K59" s="12">
-        <f t="shared" ref="K59:K60" si="116">J59</f>
+        <f t="shared" ref="K59:K93" si="116">J59</f>
         <v>0</v>
       </c>
       <c r="L59" s="15">
-        <f t="shared" ref="L59:L77" si="117">K59</f>
+        <f t="shared" ref="L59:L88" si="117">K59</f>
         <v>0</v>
       </c>
       <c r="M59" s="16">
@@ -22148,11 +22148,11 @@
         <v>0</v>
       </c>
       <c r="O59" s="12">
-        <f t="shared" ref="O59:O60" si="118">N59</f>
+        <f t="shared" ref="O59:O93" si="118">N59</f>
         <v>0</v>
       </c>
       <c r="P59" s="15">
-        <f t="shared" ref="P59:P77" si="119">O59</f>
+        <f t="shared" ref="P59:P88" si="119">O59</f>
         <v>0</v>
       </c>
       <c r="Q59" s="16">
@@ -22163,11 +22163,11 @@
         <v>3.5</v>
       </c>
       <c r="S59" s="12">
-        <f t="shared" ref="S59:S60" si="120">R59</f>
+        <f t="shared" ref="S59:S93" si="120">R59</f>
         <v>3.5</v>
       </c>
       <c r="T59" s="15">
-        <f t="shared" ref="T59:T77" si="121">S59</f>
+        <f t="shared" ref="T59:T88" si="121">S59</f>
         <v>3.5</v>
       </c>
       <c r="U59" s="16">
@@ -22175,11 +22175,11 @@
         <v>0</v>
       </c>
       <c r="W59" s="12">
-        <f t="shared" ref="W59:W60" si="122">V59</f>
+        <f t="shared" ref="W59:W93" si="122">V59</f>
         <v>0</v>
       </c>
       <c r="X59" s="15">
-        <f t="shared" ref="X59:X77" si="123">W59</f>
+        <f t="shared" ref="X59:X88" si="123">W59</f>
         <v>0</v>
       </c>
       <c r="Y59" s="16">
@@ -22187,11 +22187,11 @@
         <v>0</v>
       </c>
       <c r="AA59" s="12">
-        <f t="shared" ref="AA59:AA60" si="124">Z59</f>
+        <f t="shared" ref="AA59:AA93" si="124">Z59</f>
         <v>0</v>
       </c>
       <c r="AB59" s="15">
-        <f t="shared" ref="AB59:AB77" si="125">AA59</f>
+        <f t="shared" ref="AB59:AB88" si="125">AA59</f>
         <v>0</v>
       </c>
       <c r="AC59" s="16">
@@ -22412,7 +22412,7 @@
         <v>9.6</v>
       </c>
       <c r="K62" s="12">
-        <f t="shared" ref="K62:K67" si="126">J62</f>
+        <f t="shared" ref="K62:K93" si="126">J62</f>
         <v>0</v>
       </c>
       <c r="L62" s="15">
@@ -22424,7 +22424,7 @@
         <v>0</v>
       </c>
       <c r="O62" s="12">
-        <f t="shared" ref="O62:O67" si="127">N62</f>
+        <f t="shared" ref="O62:O93" si="127">N62</f>
         <v>0</v>
       </c>
       <c r="P62" s="15">
@@ -22439,7 +22439,7 @@
         <v>3.5</v>
       </c>
       <c r="S62" s="12">
-        <f t="shared" ref="S62:S67" si="128">R62</f>
+        <f t="shared" ref="S62:S93" si="128">R62</f>
         <v>3.5</v>
       </c>
       <c r="T62" s="15">
@@ -22454,7 +22454,7 @@
         <v>10</v>
       </c>
       <c r="W62" s="12">
-        <f t="shared" ref="W62:W67" si="129">V62</f>
+        <f t="shared" ref="W62:W93" si="129">V62</f>
         <v>10</v>
       </c>
       <c r="X62" s="15">
@@ -22469,7 +22469,7 @@
         <v>10</v>
       </c>
       <c r="AA62" s="12">
-        <f t="shared" ref="AA62:AA67" si="130">Z62</f>
+        <f t="shared" ref="AA62:AA93" si="130">Z62</f>
         <v>10</v>
       </c>
       <c r="AB62" s="15">
@@ -22875,7 +22875,7 @@
         <v>0</v>
       </c>
       <c r="M67" s="16">
-        <f t="shared" ref="M67:M77" si="132">L67</f>
+        <f t="shared" ref="M67:M93" si="132">L67</f>
         <v>0</v>
       </c>
       <c r="O67" s="12">
@@ -22887,7 +22887,7 @@
         <v>0</v>
       </c>
       <c r="Q67" s="16">
-        <f t="shared" ref="Q67:Q77" si="133">P67</f>
+        <f t="shared" ref="Q67:Q93" si="133">P67</f>
         <v>0</v>
       </c>
       <c r="S67" s="12">
@@ -22899,7 +22899,7 @@
         <v>0</v>
       </c>
       <c r="U67" s="16">
-        <f t="shared" ref="U67:U77" si="134">T67</f>
+        <f t="shared" ref="U67:U93" si="134">T67</f>
         <v>0</v>
       </c>
       <c r="W67" s="12">
@@ -22911,7 +22911,7 @@
         <v>0</v>
       </c>
       <c r="Y67" s="16">
-        <f t="shared" ref="Y67:Y77" si="135">X67</f>
+        <f t="shared" ref="Y67:Y93" si="135">X67</f>
         <v>0</v>
       </c>
       <c r="AA67" s="12">
@@ -22923,7 +22923,7 @@
         <v>0</v>
       </c>
       <c r="AC67" s="16">
-        <f t="shared" ref="AC67:AC77" si="136">AB67</f>
+        <f t="shared" ref="AC67:AC93" si="136">AB67</f>
         <v>0</v>
       </c>
     </row>
@@ -23263,7 +23263,7 @@
         <v>0</v>
       </c>
       <c r="K71" s="12">
-        <f t="shared" ref="K71:K77" si="143">J71</f>
+        <f t="shared" ref="K71:K93" si="143">J71</f>
         <v>0</v>
       </c>
       <c r="L71" s="15">
@@ -23275,7 +23275,7 @@
         <v>0</v>
       </c>
       <c r="O71" s="12">
-        <f t="shared" ref="O71:O77" si="144">N71</f>
+        <f t="shared" ref="O71:O93" si="144">N71</f>
         <v>0</v>
       </c>
       <c r="P71" s="15">
@@ -23287,7 +23287,7 @@
         <v>0</v>
       </c>
       <c r="S71" s="12">
-        <f t="shared" ref="S71:S77" si="145">R71</f>
+        <f t="shared" ref="S71:S93" si="145">R71</f>
         <v>0</v>
       </c>
       <c r="T71" s="15">
@@ -23302,7 +23302,7 @@
         <v>90</v>
       </c>
       <c r="W71" s="12">
-        <f t="shared" ref="W71:W77" si="146">V71</f>
+        <f t="shared" ref="W71:W93" si="146">V71</f>
         <v>90</v>
       </c>
       <c r="X71" s="15">
@@ -23314,7 +23314,7 @@
         <v>90</v>
       </c>
       <c r="AA71" s="12">
-        <f t="shared" ref="AA71:AA77" si="147">Z71</f>
+        <f t="shared" ref="AA71:AA93" si="147">Z71</f>
         <v>0</v>
       </c>
       <c r="AB71" s="15">
@@ -24081,7 +24081,7 @@
         <v>1</v>
       </c>
       <c r="M80" s="16">
-        <f t="shared" ref="M80:M81" si="154">L80</f>
+        <f t="shared" ref="M80:M93" si="154">L80</f>
         <v>1</v>
       </c>
       <c r="N80" s="11">
@@ -24096,7 +24096,7 @@
         <v>2.5</v>
       </c>
       <c r="Q80" s="16">
-        <f t="shared" ref="Q80:Q81" si="155">P80</f>
+        <f t="shared" ref="Q80:Q93" si="155">P80</f>
         <v>2.5</v>
       </c>
       <c r="R80" s="11">
@@ -24111,7 +24111,7 @@
         <v>1</v>
       </c>
       <c r="U80" s="16">
-        <f t="shared" ref="U80:U81" si="156">T80</f>
+        <f t="shared" ref="U80:U93" si="156">T80</f>
         <v>1</v>
       </c>
       <c r="V80" s="11">
@@ -24126,7 +24126,7 @@
         <v>1.5</v>
       </c>
       <c r="Y80" s="16">
-        <f t="shared" ref="Y80:Y81" si="157">X80</f>
+        <f t="shared" ref="Y80:Y93" si="157">X80</f>
         <v>1.5</v>
       </c>
       <c r="Z80" s="11">
@@ -24141,7 +24141,7 @@
         <v>2</v>
       </c>
       <c r="AC80" s="16">
-        <f t="shared" ref="AC80:AC81" si="158">AB80</f>
+        <f t="shared" ref="AC80:AC93" si="158">AB80</f>
         <v>2</v>
       </c>
     </row>
@@ -24944,7 +24944,7 @@
         <v>0</v>
       </c>
       <c r="K89" s="12">
-        <f t="shared" ref="K89:K90" si="169">J89</f>
+        <f t="shared" ref="K89:K93" si="169">J89</f>
         <v>0</v>
       </c>
       <c r="L89" s="15">
@@ -24956,7 +24956,7 @@
         <v>0</v>
       </c>
       <c r="O89" s="12">
-        <f t="shared" ref="O89:O90" si="170">N89</f>
+        <f t="shared" ref="O89:O93" si="170">N89</f>
         <v>0</v>
       </c>
       <c r="P89" s="15">
@@ -24968,7 +24968,7 @@
         <v>0</v>
       </c>
       <c r="S89" s="12">
-        <f t="shared" ref="S89:S90" si="171">R89</f>
+        <f t="shared" ref="S89:S93" si="171">R89</f>
         <v>0</v>
       </c>
       <c r="T89" s="15">
@@ -24980,7 +24980,7 @@
         <v>0</v>
       </c>
       <c r="W89" s="12">
-        <f t="shared" ref="W89:W90" si="172">V89</f>
+        <f t="shared" ref="W89:W93" si="172">V89</f>
         <v>0</v>
       </c>
       <c r="X89" s="15">
@@ -24992,7 +24992,7 @@
         <v>0</v>
       </c>
       <c r="AA89" s="12">
-        <f t="shared" ref="AA89:AA90" si="173">Z89</f>
+        <f t="shared" ref="AA89:AA93" si="173">Z89</f>
         <v>0</v>
       </c>
       <c r="AB89" s="15">
@@ -25360,8 +25360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView topLeftCell="L1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25795,7 +25795,7 @@
         <v>100</v>
       </c>
       <c r="K5" s="12">
-        <f t="shared" ref="K5" si="7">J5</f>
+        <f t="shared" ref="K5:K20" si="7">J5</f>
         <v>0</v>
       </c>
       <c r="L5" s="15">
@@ -25807,7 +25807,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="12">
-        <f t="shared" ref="O5" si="9">N5</f>
+        <f t="shared" ref="O5:O20" si="9">N5</f>
         <v>0</v>
       </c>
       <c r="P5" s="15">
@@ -25822,7 +25822,7 @@
         <v>25</v>
       </c>
       <c r="S5" s="12">
-        <f t="shared" ref="S5" si="11">R5</f>
+        <f t="shared" ref="S5:S20" si="11">R5</f>
         <v>25</v>
       </c>
       <c r="T5" s="15">
@@ -25837,7 +25837,7 @@
         <v>60</v>
       </c>
       <c r="W5" s="12">
-        <f t="shared" ref="W5" si="13">V5</f>
+        <f t="shared" ref="W5:W20" si="13">V5</f>
         <v>60</v>
       </c>
       <c r="X5" s="15">
@@ -25852,7 +25852,7 @@
         <v>78</v>
       </c>
       <c r="AA5" s="12">
-        <f t="shared" ref="AA5" si="15">Z5</f>
+        <f t="shared" ref="AA5:AA20" si="15">Z5</f>
         <v>78</v>
       </c>
       <c r="AB5" s="15">
@@ -26262,7 +26262,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="12">
-        <f t="shared" ref="K10" si="17">J10</f>
+        <f t="shared" ref="K10:K25" si="17">J10</f>
         <v>0</v>
       </c>
       <c r="L10" s="15">
@@ -26274,7 +26274,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="12">
-        <f t="shared" ref="O10" si="18">N10</f>
+        <f t="shared" ref="O10:O25" si="18">N10</f>
         <v>0</v>
       </c>
       <c r="P10" s="15">
@@ -26286,7 +26286,7 @@
         <v>0</v>
       </c>
       <c r="S10" s="12">
-        <f t="shared" ref="S10" si="19">R10</f>
+        <f t="shared" ref="S10:S25" si="19">R10</f>
         <v>0</v>
       </c>
       <c r="T10" s="15">
@@ -26301,7 +26301,7 @@
         <v>44</v>
       </c>
       <c r="W10" s="12">
-        <f t="shared" ref="W10" si="20">V10</f>
+        <f t="shared" ref="W10:W25" si="20">V10</f>
         <v>44</v>
       </c>
       <c r="X10" s="15">
@@ -26313,7 +26313,7 @@
         <v>44</v>
       </c>
       <c r="AA10" s="12">
-        <f t="shared" ref="AA10" si="21">Z10</f>
+        <f t="shared" ref="AA10:AA25" si="21">Z10</f>
         <v>0</v>
       </c>
       <c r="AB10" s="15">
@@ -28468,7 +28468,7 @@
         <v>5</v>
       </c>
       <c r="M34" s="16">
-        <f t="shared" ref="M34" si="41">L34</f>
+        <f t="shared" ref="M34:M47" si="41">L34</f>
         <v>5</v>
       </c>
       <c r="N34" s="11">
@@ -28483,7 +28483,7 @@
         <v>3</v>
       </c>
       <c r="Q34" s="16">
-        <f t="shared" ref="Q34" si="42">P34</f>
+        <f t="shared" ref="Q34:Q47" si="42">P34</f>
         <v>3</v>
       </c>
       <c r="R34" s="11">
@@ -28498,7 +28498,7 @@
         <v>5</v>
       </c>
       <c r="U34" s="16">
-        <f t="shared" ref="U34" si="43">T34</f>
+        <f t="shared" ref="U34:U47" si="43">T34</f>
         <v>5</v>
       </c>
       <c r="V34" s="11">
@@ -28513,7 +28513,7 @@
         <v>6</v>
       </c>
       <c r="Y34" s="16">
-        <f t="shared" ref="Y34" si="44">X34</f>
+        <f t="shared" ref="Y34:Y47" si="44">X34</f>
         <v>6</v>
       </c>
       <c r="Z34" s="11">
@@ -28528,7 +28528,7 @@
         <v>5</v>
       </c>
       <c r="AC34" s="16">
-        <f t="shared" ref="AC34" si="45">AB34</f>
+        <f t="shared" ref="AC34:AC47" si="45">AB34</f>
         <v>5</v>
       </c>
     </row>
@@ -28558,7 +28558,7 @@
         <v>5.4</v>
       </c>
       <c r="H35" s="15">
-        <f>G35*$D35</f>
+        <f>MIN(100,G35*$D35)</f>
         <v>8.1000000000000014</v>
       </c>
       <c r="I35" s="16">
@@ -28573,7 +28573,7 @@
         <v>17.5</v>
       </c>
       <c r="L35" s="15">
-        <f>K35*$D35</f>
+        <f>MIN(100,K35*$D35)</f>
         <v>26.25</v>
       </c>
       <c r="M35" s="16">
@@ -28588,7 +28588,7 @@
         <v>0.5</v>
       </c>
       <c r="P35" s="15">
-        <f>O35*$D35</f>
+        <f>MIN(100,O35*$D35)</f>
         <v>0.75</v>
       </c>
       <c r="Q35" s="16">
@@ -28603,7 +28603,7 @@
         <v>2.5</v>
       </c>
       <c r="T35" s="15">
-        <f>S35*$D35</f>
+        <f>MIN(100,S35*$D35)</f>
         <v>3.75</v>
       </c>
       <c r="U35" s="16">
@@ -28618,7 +28618,7 @@
         <v>7.5</v>
       </c>
       <c r="X35" s="15">
-        <f>W35*$D35</f>
+        <f>MIN(100,W35*$D35)</f>
         <v>11.25</v>
       </c>
       <c r="Y35" s="16">
@@ -28633,7 +28633,7 @@
         <v>20</v>
       </c>
       <c r="AB35" s="15">
-        <f>AA35*$D35</f>
+        <f>MIN(100,AA35*$D35)</f>
         <v>30</v>
       </c>
       <c r="AC35" s="16">
@@ -28778,66 +28778,66 @@
         <v>2</v>
       </c>
       <c r="K37" s="12">
-        <f t="shared" ref="K37" si="47">J37</f>
+        <f t="shared" ref="K37:K44" si="47">J37</f>
         <v>2</v>
       </c>
       <c r="L37" s="15">
-        <f t="shared" ref="L37" si="48">K37</f>
+        <f t="shared" ref="L37:L44" si="48">K37</f>
         <v>2</v>
       </c>
       <c r="M37" s="16">
-        <f t="shared" ref="M37" si="49">L37</f>
+        <f t="shared" ref="M37:M50" si="49">L37</f>
         <v>2</v>
       </c>
       <c r="O37" s="12">
-        <f t="shared" ref="O37" si="50">N37</f>
+        <f t="shared" ref="O37:O44" si="50">N37</f>
         <v>0</v>
       </c>
       <c r="P37" s="15">
-        <f t="shared" ref="P37" si="51">O37</f>
+        <f t="shared" ref="P37:P44" si="51">O37</f>
         <v>0</v>
       </c>
       <c r="Q37" s="16">
-        <f t="shared" ref="Q37" si="52">P37</f>
+        <f t="shared" ref="Q37:Q50" si="52">P37</f>
         <v>0</v>
       </c>
       <c r="R37" s="11">
         <v>1</v>
       </c>
       <c r="S37" s="12">
-        <f t="shared" ref="S37" si="53">R37</f>
+        <f t="shared" ref="S37:S44" si="53">R37</f>
         <v>1</v>
       </c>
       <c r="T37" s="15">
-        <f t="shared" ref="T37" si="54">S37</f>
+        <f t="shared" ref="T37:T44" si="54">S37</f>
         <v>1</v>
       </c>
       <c r="U37" s="16">
-        <f t="shared" ref="U37" si="55">T37</f>
+        <f t="shared" ref="U37:U50" si="55">T37</f>
         <v>1</v>
       </c>
       <c r="W37" s="12">
-        <f t="shared" ref="W37" si="56">V37</f>
+        <f t="shared" ref="W37:W44" si="56">V37</f>
         <v>0</v>
       </c>
       <c r="X37" s="15">
-        <f t="shared" ref="X37" si="57">W37</f>
+        <f t="shared" ref="X37:X44" si="57">W37</f>
         <v>0</v>
       </c>
       <c r="Y37" s="16">
-        <f t="shared" ref="Y37" si="58">X37</f>
+        <f t="shared" ref="Y37:Y50" si="58">X37</f>
         <v>0</v>
       </c>
       <c r="AA37" s="12">
-        <f t="shared" ref="AA37" si="59">Z37</f>
+        <f t="shared" ref="AA37:AA44" si="59">Z37</f>
         <v>0</v>
       </c>
       <c r="AB37" s="15">
-        <f t="shared" ref="AB37" si="60">AA37</f>
+        <f t="shared" ref="AB37:AB44" si="60">AA37</f>
         <v>0</v>
       </c>
       <c r="AC37" s="16">
-        <f t="shared" ref="AC37" si="61">AB37</f>
+        <f t="shared" ref="AC37:AC50" si="61">AB37</f>
         <v>0</v>
       </c>
     </row>
@@ -28867,7 +28867,7 @@
         <v>0.3</v>
       </c>
       <c r="H38" s="15">
-        <f>G38*$D38</f>
+        <f>MIN(100,G38*$D38)</f>
         <v>0.44999999999999996</v>
       </c>
       <c r="I38" s="16">
@@ -28882,7 +28882,7 @@
         <v>1.25</v>
       </c>
       <c r="L38" s="15">
-        <f>K38*$D38</f>
+        <f>MIN(100,K38*$D38)</f>
         <v>1.875</v>
       </c>
       <c r="M38" s="16">
@@ -28894,7 +28894,7 @@
         <v>0</v>
       </c>
       <c r="P38" s="15">
-        <f>O38*$D38</f>
+        <f>MIN(100,O38*$D38)</f>
         <v>0</v>
       </c>
       <c r="Q38" s="16">
@@ -28909,7 +28909,7 @@
         <v>5</v>
       </c>
       <c r="T38" s="15">
-        <f>S38*$D38</f>
+        <f>MIN(100,S38*$D38)</f>
         <v>7.5</v>
       </c>
       <c r="U38" s="16">
@@ -28921,7 +28921,7 @@
         <v>0</v>
       </c>
       <c r="X38" s="15">
-        <f>W38*$D38</f>
+        <f>MIN(100,W38*$D38)</f>
         <v>0</v>
       </c>
       <c r="Y38" s="16">
@@ -28933,7 +28933,7 @@
         <v>0</v>
       </c>
       <c r="AB38" s="15">
-        <f>AA38*$D38</f>
+        <f>MIN(100,AA38*$D38)</f>
         <v>0</v>
       </c>
       <c r="AC38" s="16">
@@ -29066,75 +29066,75 @@
         <v>0.9</v>
       </c>
       <c r="K40" s="12">
-        <f t="shared" ref="K40" si="62">J40</f>
+        <f t="shared" ref="K40:K47" si="62">J40</f>
         <v>0</v>
       </c>
       <c r="L40" s="15">
-        <f t="shared" ref="L40" si="63">K40</f>
+        <f t="shared" ref="L40:L47" si="63">K40</f>
         <v>0</v>
       </c>
       <c r="M40" s="16">
-        <f t="shared" ref="M40" si="64">L40</f>
+        <f t="shared" ref="M40:M53" si="64">L40</f>
         <v>0</v>
       </c>
       <c r="N40" s="11">
         <v>2</v>
       </c>
       <c r="O40" s="12">
-        <f t="shared" ref="O40" si="65">N40</f>
+        <f t="shared" ref="O40:O47" si="65">N40</f>
         <v>2</v>
       </c>
       <c r="P40" s="15">
-        <f t="shared" ref="P40" si="66">O40</f>
+        <f t="shared" ref="P40:P47" si="66">O40</f>
         <v>2</v>
       </c>
       <c r="Q40" s="16">
-        <f t="shared" ref="Q40" si="67">P40</f>
+        <f t="shared" ref="Q40:Q53" si="67">P40</f>
         <v>2</v>
       </c>
       <c r="R40" s="11">
         <v>1</v>
       </c>
       <c r="S40" s="12">
-        <f t="shared" ref="S40" si="68">R40</f>
+        <f t="shared" ref="S40:S47" si="68">R40</f>
         <v>1</v>
       </c>
       <c r="T40" s="15">
-        <f t="shared" ref="T40" si="69">S40</f>
+        <f t="shared" ref="T40:T47" si="69">S40</f>
         <v>1</v>
       </c>
       <c r="U40" s="16">
-        <f t="shared" ref="U40" si="70">T40</f>
+        <f t="shared" ref="U40:U53" si="70">T40</f>
         <v>1</v>
       </c>
       <c r="V40" s="11">
         <v>2.5</v>
       </c>
       <c r="W40" s="12">
-        <f t="shared" ref="W40" si="71">V40</f>
+        <f t="shared" ref="W40:W47" si="71">V40</f>
         <v>2.5</v>
       </c>
       <c r="X40" s="15">
-        <f t="shared" ref="X40" si="72">W40</f>
+        <f t="shared" ref="X40:X47" si="72">W40</f>
         <v>2.5</v>
       </c>
       <c r="Y40" s="16">
-        <f t="shared" ref="Y40" si="73">X40</f>
+        <f t="shared" ref="Y40:Y53" si="73">X40</f>
         <v>2.5</v>
       </c>
       <c r="Z40" s="11">
         <v>2</v>
       </c>
       <c r="AA40" s="12">
-        <f t="shared" ref="AA40" si="74">Z40</f>
+        <f t="shared" ref="AA40:AA47" si="74">Z40</f>
         <v>2</v>
       </c>
       <c r="AB40" s="15">
-        <f t="shared" ref="AB40" si="75">AA40</f>
+        <f t="shared" ref="AB40:AB47" si="75">AA40</f>
         <v>2</v>
       </c>
       <c r="AC40" s="16">
-        <f t="shared" ref="AC40" si="76">AB40</f>
+        <f t="shared" ref="AC40:AC53" si="76">AB40</f>
         <v>2</v>
       </c>
     </row>
@@ -29270,7 +29270,7 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="H42" s="15">
-        <f>G42*$D42</f>
+        <f>MIN(100,G42*$D42)</f>
         <v>0.26249999999999996</v>
       </c>
       <c r="I42" s="16">
@@ -29282,7 +29282,7 @@
         <v>0</v>
       </c>
       <c r="L42" s="15">
-        <f>K42*$D42</f>
+        <f>MIN(100,K42*$D42)</f>
         <v>0</v>
       </c>
       <c r="M42" s="16">
@@ -29297,7 +29297,7 @@
         <v>22.5</v>
       </c>
       <c r="P42" s="15">
-        <f>O42*$D42</f>
+        <f>MIN(100,O42*$D42)</f>
         <v>33.75</v>
       </c>
       <c r="Q42" s="16">
@@ -29312,7 +29312,7 @@
         <v>0.5</v>
       </c>
       <c r="T42" s="15">
-        <f>S42*$D42</f>
+        <f>MIN(100,S42*$D42)</f>
         <v>0.75</v>
       </c>
       <c r="U42" s="16">
@@ -29327,7 +29327,7 @@
         <v>7.5</v>
       </c>
       <c r="X42" s="15">
-        <f>W42*$D42</f>
+        <f>MIN(100,W42*$D42)</f>
         <v>11.25</v>
       </c>
       <c r="Y42" s="16">
@@ -29342,7 +29342,7 @@
         <v>5</v>
       </c>
       <c r="AB42" s="15">
-        <f>AA42*$D42</f>
+        <f>MIN(100,AA42*$D42)</f>
         <v>7.5</v>
       </c>
       <c r="AC42" s="16">
@@ -29485,11 +29485,11 @@
         <v>0</v>
       </c>
       <c r="L44" s="15">
-        <f t="shared" ref="L44" si="77">K44</f>
+        <f t="shared" ref="L44:L51" si="77">K44</f>
         <v>0</v>
       </c>
       <c r="M44" s="16">
-        <f t="shared" ref="M44" si="78">L44</f>
+        <f t="shared" ref="M44:M57" si="78">L44</f>
         <v>0</v>
       </c>
       <c r="N44" s="11">
@@ -29500,11 +29500,11 @@
         <v>1</v>
       </c>
       <c r="P44" s="15">
-        <f t="shared" ref="P44" si="79">O44</f>
+        <f t="shared" ref="P44:P51" si="79">O44</f>
         <v>1</v>
       </c>
       <c r="Q44" s="16">
-        <f t="shared" ref="Q44" si="80">P44</f>
+        <f t="shared" ref="Q44:Q57" si="80">P44</f>
         <v>1</v>
       </c>
       <c r="R44" s="11">
@@ -29515,11 +29515,11 @@
         <v>0.5</v>
       </c>
       <c r="T44" s="15">
-        <f t="shared" ref="T44" si="81">S44</f>
+        <f t="shared" ref="T44:T51" si="81">S44</f>
         <v>0.5</v>
       </c>
       <c r="U44" s="16">
-        <f t="shared" ref="U44" si="82">T44</f>
+        <f t="shared" ref="U44:U57" si="82">T44</f>
         <v>0.5</v>
       </c>
       <c r="W44" s="12">
@@ -29527,11 +29527,11 @@
         <v>0</v>
       </c>
       <c r="X44" s="15">
-        <f t="shared" ref="X44" si="83">W44</f>
+        <f t="shared" ref="X44:X51" si="83">W44</f>
         <v>0</v>
       </c>
       <c r="Y44" s="16">
-        <f t="shared" ref="Y44" si="84">X44</f>
+        <f t="shared" ref="Y44:Y57" si="84">X44</f>
         <v>0</v>
       </c>
       <c r="Z44" s="11">
@@ -29542,11 +29542,11 @@
         <v>1</v>
       </c>
       <c r="AB44" s="15">
-        <f t="shared" ref="AB44" si="85">AA44</f>
+        <f t="shared" ref="AB44:AB51" si="85">AA44</f>
         <v>1</v>
       </c>
       <c r="AC44" s="16">
-        <f t="shared" ref="AC44" si="86">AB44</f>
+        <f t="shared" ref="AC44:AC57" si="86">AB44</f>
         <v>1</v>
       </c>
     </row>
@@ -29679,7 +29679,7 @@
         <v>0.05</v>
       </c>
       <c r="H46" s="15">
-        <f>G46*$D46</f>
+        <f>MIN(100,G46*$D46)</f>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="I46" s="16">
@@ -29691,7 +29691,7 @@
         <v>0</v>
       </c>
       <c r="L46" s="15">
-        <f>K46*$D46</f>
+        <f>MIN(100,K46*$D46)</f>
         <v>0</v>
       </c>
       <c r="M46" s="16">
@@ -29706,7 +29706,7 @@
         <v>2</v>
       </c>
       <c r="P46" s="15">
-        <f>O46*$D46</f>
+        <f>MIN(100,O46*$D46)</f>
         <v>3</v>
       </c>
       <c r="Q46" s="16">
@@ -29721,7 +29721,7 @@
         <v>1.25</v>
       </c>
       <c r="T46" s="15">
-        <f>S46*$D46</f>
+        <f>MIN(100,S46*$D46)</f>
         <v>1.875</v>
       </c>
       <c r="U46" s="16">
@@ -29733,7 +29733,7 @@
         <v>0</v>
       </c>
       <c r="X46" s="15">
-        <f>W46*$D46</f>
+        <f>MIN(100,W46*$D46)</f>
         <v>0</v>
       </c>
       <c r="Y46" s="16">
@@ -29748,7 +29748,7 @@
         <v>5</v>
       </c>
       <c r="AB46" s="15">
-        <f>AA46*$D46</f>
+        <f>MIN(100,AA46*$D46)</f>
         <v>7.5</v>
       </c>
       <c r="AC46" s="16">
@@ -29796,7 +29796,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="16">
-        <f t="shared" ref="M47" si="93">L47</f>
+        <f t="shared" ref="M47:M60" si="93">L47</f>
         <v>0</v>
       </c>
       <c r="N47" s="11">
@@ -29811,7 +29811,7 @@
         <v>70</v>
       </c>
       <c r="Q47" s="16">
-        <f t="shared" ref="Q47" si="94">P47</f>
+        <f t="shared" ref="Q47:Q60" si="94">P47</f>
         <v>70</v>
       </c>
       <c r="R47" s="11">
@@ -29826,7 +29826,7 @@
         <v>90</v>
       </c>
       <c r="U47" s="16">
-        <f t="shared" ref="U47" si="95">T47</f>
+        <f t="shared" ref="U47:U60" si="95">T47</f>
         <v>90</v>
       </c>
       <c r="W47" s="12">
@@ -29838,7 +29838,7 @@
         <v>0</v>
       </c>
       <c r="Y47" s="16">
-        <f t="shared" ref="Y47" si="96">X47</f>
+        <f t="shared" ref="Y47:Y60" si="96">X47</f>
         <v>0</v>
       </c>
       <c r="Z47" s="11">
@@ -29853,7 +29853,7 @@
         <v>60</v>
       </c>
       <c r="AC47" s="16">
-        <f t="shared" ref="AC47" si="97">AB47</f>
+        <f t="shared" ref="AC47:AC60" si="97">AB47</f>
         <v>60</v>
       </c>
     </row>
@@ -31016,7 +31016,7 @@
         <v>9.6</v>
       </c>
       <c r="K59" s="12">
-        <f t="shared" ref="K59:K60" si="106">J59</f>
+        <f t="shared" ref="K59:K93" si="106">J59</f>
         <v>0</v>
       </c>
       <c r="L59" s="15">
@@ -31028,7 +31028,7 @@
         <v>0</v>
       </c>
       <c r="O59" s="12">
-        <f t="shared" ref="O59:O60" si="108">N59</f>
+        <f t="shared" ref="O59:O93" si="108">N59</f>
         <v>0</v>
       </c>
       <c r="P59" s="15">
@@ -31043,7 +31043,7 @@
         <v>3.5</v>
       </c>
       <c r="S59" s="12">
-        <f t="shared" ref="S59:S60" si="110">R59</f>
+        <f t="shared" ref="S59:S93" si="110">R59</f>
         <v>3.5</v>
       </c>
       <c r="T59" s="15">
@@ -31055,7 +31055,7 @@
         <v>3.5</v>
       </c>
       <c r="W59" s="12">
-        <f t="shared" ref="W59:W60" si="112">V59</f>
+        <f t="shared" ref="W59:W93" si="112">V59</f>
         <v>0</v>
       </c>
       <c r="X59" s="15">
@@ -31067,7 +31067,7 @@
         <v>0</v>
       </c>
       <c r="AA59" s="12">
-        <f t="shared" ref="AA59:AA60" si="114">Z59</f>
+        <f t="shared" ref="AA59:AA93" si="114">Z59</f>
         <v>0</v>
       </c>
       <c r="AB59" s="15">
@@ -31290,7 +31290,7 @@
         <v>9.6</v>
       </c>
       <c r="K62" s="12">
-        <f t="shared" ref="K62:K67" si="116">J62</f>
+        <f t="shared" ref="K62:K93" si="116">J62</f>
         <v>0</v>
       </c>
       <c r="L62" s="15">
@@ -31302,7 +31302,7 @@
         <v>0</v>
       </c>
       <c r="O62" s="12">
-        <f t="shared" ref="O62:O67" si="117">N62</f>
+        <f t="shared" ref="O62:O93" si="117">N62</f>
         <v>0</v>
       </c>
       <c r="P62" s="15">
@@ -31317,7 +31317,7 @@
         <v>3.5</v>
       </c>
       <c r="S62" s="12">
-        <f t="shared" ref="S62:S67" si="118">R62</f>
+        <f t="shared" ref="S62:S93" si="118">R62</f>
         <v>3.5</v>
       </c>
       <c r="T62" s="15">
@@ -31332,7 +31332,7 @@
         <v>10</v>
       </c>
       <c r="W62" s="12">
-        <f t="shared" ref="W62:W67" si="119">V62</f>
+        <f t="shared" ref="W62:W93" si="119">V62</f>
         <v>10</v>
       </c>
       <c r="X62" s="15">
@@ -31347,7 +31347,7 @@
         <v>10</v>
       </c>
       <c r="AA62" s="12">
-        <f t="shared" ref="AA62:AA67" si="120">Z62</f>
+        <f t="shared" ref="AA62:AA93" si="120">Z62</f>
         <v>10</v>
       </c>
       <c r="AB62" s="15">
@@ -32141,7 +32141,7 @@
         <v>0</v>
       </c>
       <c r="K71" s="12">
-        <f t="shared" ref="K71:K77" si="133">J71</f>
+        <f t="shared" ref="K71:K93" si="133">J71</f>
         <v>0</v>
       </c>
       <c r="L71" s="15">
@@ -32153,7 +32153,7 @@
         <v>0</v>
       </c>
       <c r="O71" s="12">
-        <f t="shared" ref="O71:O77" si="134">N71</f>
+        <f t="shared" ref="O71:O93" si="134">N71</f>
         <v>0</v>
       </c>
       <c r="P71" s="15">
@@ -32165,7 +32165,7 @@
         <v>0</v>
       </c>
       <c r="S71" s="12">
-        <f t="shared" ref="S71:S77" si="135">R71</f>
+        <f t="shared" ref="S71:S93" si="135">R71</f>
         <v>0</v>
       </c>
       <c r="T71" s="15">
@@ -32180,7 +32180,7 @@
         <v>90</v>
       </c>
       <c r="W71" s="12">
-        <f t="shared" ref="W71:W77" si="136">V71</f>
+        <f t="shared" ref="W71:W93" si="136">V71</f>
         <v>90</v>
       </c>
       <c r="X71" s="15">
@@ -32192,7 +32192,7 @@
         <v>90</v>
       </c>
       <c r="AA71" s="12">
-        <f t="shared" ref="AA71:AA77" si="137">Z71</f>
+        <f t="shared" ref="AA71:AA93" si="137">Z71</f>
         <v>0</v>
       </c>
       <c r="AB71" s="15">
@@ -32849,7 +32849,7 @@
         <v>0</v>
       </c>
       <c r="H79" s="15">
-        <f t="shared" si="139"/>
+        <f>MIN(100,G79*$D79)</f>
         <v>0</v>
       </c>
       <c r="I79" s="16">
@@ -32861,7 +32861,7 @@
         <v>0</v>
       </c>
       <c r="L79" s="15">
-        <f t="shared" si="141"/>
+        <f>MIN(100,K79*$D79)</f>
         <v>0</v>
       </c>
       <c r="M79" s="16">
@@ -32873,7 +32873,7 @@
         <v>0</v>
       </c>
       <c r="P79" s="15">
-        <f t="shared" si="143"/>
+        <f>MIN(100,O79*$D79)</f>
         <v>0</v>
       </c>
       <c r="Q79" s="16">
@@ -32888,7 +32888,7 @@
         <v>2.5</v>
       </c>
       <c r="T79" s="15">
-        <f t="shared" si="145"/>
+        <f>MIN(100,S79*$D79)</f>
         <v>3.75</v>
       </c>
       <c r="U79" s="16">
@@ -32900,7 +32900,7 @@
         <v>0</v>
       </c>
       <c r="X79" s="15">
-        <f t="shared" si="147"/>
+        <f>MIN(100,W79*$D79)</f>
         <v>0</v>
       </c>
       <c r="Y79" s="16">
@@ -32912,7 +32912,7 @@
         <v>0</v>
       </c>
       <c r="AB79" s="15">
-        <f t="shared" si="149"/>
+        <f>MIN(100,AA79*$D79)</f>
         <v>0</v>
       </c>
       <c r="AC79" s="16">
@@ -32959,7 +32959,7 @@
         <v>0.5</v>
       </c>
       <c r="L80" s="15">
-        <f t="shared" si="141"/>
+        <f t="shared" ref="L80:L85" si="150">K80*$D80</f>
         <v>1</v>
       </c>
       <c r="M80" s="16">
@@ -32974,7 +32974,7 @@
         <v>1.25</v>
       </c>
       <c r="P80" s="15">
-        <f t="shared" si="143"/>
+        <f t="shared" ref="P80:P85" si="151">O80*$D80</f>
         <v>2.5</v>
       </c>
       <c r="Q80" s="16">
@@ -32989,7 +32989,7 @@
         <v>0.5</v>
       </c>
       <c r="T80" s="15">
-        <f t="shared" si="145"/>
+        <f t="shared" ref="T80:T85" si="152">S80*$D80</f>
         <v>1</v>
       </c>
       <c r="U80" s="16">
@@ -33004,7 +33004,7 @@
         <v>0.75</v>
       </c>
       <c r="X80" s="15">
-        <f t="shared" si="147"/>
+        <f t="shared" ref="X80:X85" si="153">W80*$D80</f>
         <v>1.5</v>
       </c>
       <c r="Y80" s="16">
@@ -33019,7 +33019,7 @@
         <v>1</v>
       </c>
       <c r="AB80" s="15">
-        <f t="shared" si="149"/>
+        <f t="shared" ref="AB80:AB85" si="154">AA80*$D80</f>
         <v>2</v>
       </c>
       <c r="AC80" s="16">
@@ -33051,7 +33051,7 @@
         <v>35</v>
       </c>
       <c r="H81" s="15">
-        <f t="shared" si="139"/>
+        <f>MIN(100,G81*$D81)</f>
         <v>70</v>
       </c>
       <c r="I81" s="16">
@@ -33066,7 +33066,7 @@
         <v>30</v>
       </c>
       <c r="L81" s="15">
-        <f t="shared" si="141"/>
+        <f>MIN(100,K81*$D81)</f>
         <v>60</v>
       </c>
       <c r="M81" s="16">
@@ -33081,7 +33081,7 @@
         <v>2.5</v>
       </c>
       <c r="P81" s="15">
-        <f t="shared" si="143"/>
+        <f>MIN(100,O81*$D81)</f>
         <v>5</v>
       </c>
       <c r="Q81" s="16">
@@ -33096,7 +33096,7 @@
         <v>7.5</v>
       </c>
       <c r="T81" s="15">
-        <f t="shared" si="145"/>
+        <f>MIN(100,S81*$D81)</f>
         <v>15</v>
       </c>
       <c r="U81" s="16">
@@ -33111,7 +33111,7 @@
         <v>45</v>
       </c>
       <c r="X81" s="15">
-        <f t="shared" si="147"/>
+        <f>MIN(100,W81*$D81)</f>
         <v>90</v>
       </c>
       <c r="Y81" s="16">
@@ -33126,7 +33126,7 @@
         <v>35</v>
       </c>
       <c r="AB81" s="15">
-        <f t="shared" si="149"/>
+        <f>MIN(100,AA81*$D81)</f>
         <v>70</v>
       </c>
       <c r="AC81" s="16">
@@ -33169,7 +33169,7 @@
         <v>0</v>
       </c>
       <c r="L82" s="15">
-        <f t="shared" si="141"/>
+        <f t="shared" ref="L82:L87" si="155">K82*$D82</f>
         <v>0</v>
       </c>
       <c r="M82" s="16">
@@ -33181,7 +33181,7 @@
         <v>0</v>
       </c>
       <c r="P82" s="15">
-        <f t="shared" si="143"/>
+        <f t="shared" ref="P82:P87" si="156">O82*$D82</f>
         <v>0</v>
       </c>
       <c r="Q82" s="16">
@@ -33196,7 +33196,7 @@
         <v>1.25</v>
       </c>
       <c r="T82" s="15">
-        <f t="shared" si="145"/>
+        <f t="shared" ref="T82:T87" si="157">S82*$D82</f>
         <v>1.875</v>
       </c>
       <c r="U82" s="16">
@@ -33211,7 +33211,7 @@
         <v>0.5</v>
       </c>
       <c r="X82" s="15">
-        <f t="shared" si="147"/>
+        <f t="shared" ref="X82:X87" si="158">W82*$D82</f>
         <v>0.75</v>
       </c>
       <c r="Y82" s="16">
@@ -33223,7 +33223,7 @@
         <v>0</v>
       </c>
       <c r="AB82" s="15">
-        <f t="shared" si="149"/>
+        <f t="shared" ref="AB82:AB87" si="159">AA82*$D82</f>
         <v>0</v>
       </c>
       <c r="AC82" s="16">
@@ -33254,7 +33254,7 @@
         <v>0</v>
       </c>
       <c r="H83" s="15">
-        <f t="shared" si="139"/>
+        <f>MIN(100,G83*$D83)</f>
         <v>0</v>
       </c>
       <c r="I83" s="16">
@@ -33266,7 +33266,7 @@
         <v>0</v>
       </c>
       <c r="L83" s="15">
-        <f t="shared" si="141"/>
+        <f>MIN(100,K83*$D83)</f>
         <v>0</v>
       </c>
       <c r="M83" s="16">
@@ -33278,7 +33278,7 @@
         <v>0</v>
       </c>
       <c r="P83" s="15">
-        <f t="shared" si="143"/>
+        <f>MIN(100,O83*$D83)</f>
         <v>0</v>
       </c>
       <c r="Q83" s="16">
@@ -33293,7 +33293,7 @@
         <v>40</v>
       </c>
       <c r="T83" s="15">
-        <f t="shared" si="145"/>
+        <f>MIN(100,S83*$D83)</f>
         <v>60</v>
       </c>
       <c r="U83" s="16">
@@ -33308,7 +33308,7 @@
         <v>2.5</v>
       </c>
       <c r="X83" s="15">
-        <f t="shared" si="147"/>
+        <f>MIN(100,W83*$D83)</f>
         <v>3.75</v>
       </c>
       <c r="Y83" s="16">
@@ -33320,7 +33320,7 @@
         <v>0</v>
       </c>
       <c r="AB83" s="15">
-        <f t="shared" si="149"/>
+        <f>MIN(100,AA83*$D83)</f>
         <v>0</v>
       </c>
       <c r="AC83" s="16">
@@ -33350,7 +33350,7 @@
         <v>0</v>
       </c>
       <c r="I84" s="16">
-        <f t="shared" ref="I84:I93" si="150">H84</f>
+        <f t="shared" ref="I84:I93" si="160">H84</f>
         <v>0</v>
       </c>
       <c r="J84" s="11">
@@ -33361,11 +33361,11 @@
         <v>0.05</v>
       </c>
       <c r="L84" s="15">
-        <f t="shared" ref="L84:L93" si="151">K84</f>
+        <f t="shared" ref="L84:L93" si="161">K84</f>
         <v>0.05</v>
       </c>
       <c r="M84" s="16">
-        <f t="shared" ref="M84:M93" si="152">L84</f>
+        <f t="shared" ref="M84:M93" si="162">L84</f>
         <v>0.05</v>
       </c>
       <c r="O84" s="12">
@@ -33373,11 +33373,11 @@
         <v>0</v>
       </c>
       <c r="P84" s="15">
-        <f t="shared" ref="P84:P93" si="153">O84</f>
+        <f t="shared" ref="P84:P93" si="163">O84</f>
         <v>0</v>
       </c>
       <c r="Q84" s="16">
-        <f t="shared" ref="Q84:Q93" si="154">P84</f>
+        <f t="shared" ref="Q84:Q93" si="164">P84</f>
         <v>0</v>
       </c>
       <c r="R84" s="11">
@@ -33388,11 +33388,11 @@
         <v>0.5</v>
       </c>
       <c r="T84" s="15">
-        <f t="shared" ref="T84:T93" si="155">S84</f>
+        <f t="shared" ref="T84:T93" si="165">S84</f>
         <v>0.5</v>
       </c>
       <c r="U84" s="16">
-        <f t="shared" ref="U84:U93" si="156">T84</f>
+        <f t="shared" ref="U84:U93" si="166">T84</f>
         <v>0.5</v>
       </c>
       <c r="W84" s="12">
@@ -33400,11 +33400,11 @@
         <v>0</v>
       </c>
       <c r="X84" s="15">
-        <f t="shared" ref="X84:X93" si="157">W84</f>
+        <f t="shared" ref="X84:X93" si="167">W84</f>
         <v>0</v>
       </c>
       <c r="Y84" s="16">
-        <f t="shared" ref="Y84:Y93" si="158">X84</f>
+        <f t="shared" ref="Y84:Y93" si="168">X84</f>
         <v>0</v>
       </c>
       <c r="AA84" s="12">
@@ -33412,11 +33412,11 @@
         <v>0</v>
       </c>
       <c r="AB84" s="15">
-        <f t="shared" ref="AB84:AB93" si="159">AA84</f>
+        <f t="shared" ref="AB84:AB93" si="169">AA84</f>
         <v>0</v>
       </c>
       <c r="AC84" s="16">
-        <f t="shared" ref="AC84:AC93" si="160">AB84</f>
+        <f t="shared" ref="AC84:AC93" si="170">AB84</f>
         <v>0</v>
       </c>
     </row>
@@ -33442,7 +33442,7 @@
         <v>0</v>
       </c>
       <c r="I85" s="16">
-        <f t="shared" si="150"/>
+        <f t="shared" si="160"/>
         <v>0</v>
       </c>
       <c r="J85" s="11">
@@ -33453,11 +33453,11 @@
         <v>15</v>
       </c>
       <c r="L85" s="15">
-        <f t="shared" si="151"/>
+        <f t="shared" si="161"/>
         <v>15</v>
       </c>
       <c r="M85" s="16">
-        <f t="shared" si="152"/>
+        <f t="shared" si="162"/>
         <v>15</v>
       </c>
       <c r="O85" s="12">
@@ -33465,11 +33465,11 @@
         <v>0</v>
       </c>
       <c r="P85" s="15">
-        <f t="shared" si="153"/>
+        <f t="shared" si="163"/>
         <v>0</v>
       </c>
       <c r="Q85" s="16">
-        <f t="shared" si="154"/>
+        <f t="shared" si="164"/>
         <v>0</v>
       </c>
       <c r="R85" s="11">
@@ -33480,11 +33480,11 @@
         <v>22.5</v>
       </c>
       <c r="T85" s="15">
-        <f t="shared" si="155"/>
+        <f t="shared" si="165"/>
         <v>22.5</v>
       </c>
       <c r="U85" s="16">
-        <f t="shared" si="156"/>
+        <f t="shared" si="166"/>
         <v>22.5</v>
       </c>
       <c r="W85" s="12">
@@ -33492,11 +33492,11 @@
         <v>0</v>
       </c>
       <c r="X85" s="15">
-        <f t="shared" si="157"/>
+        <f t="shared" si="167"/>
         <v>0</v>
       </c>
       <c r="Y85" s="16">
-        <f t="shared" si="158"/>
+        <f t="shared" si="168"/>
         <v>0</v>
       </c>
       <c r="AA85" s="12">
@@ -33504,11 +33504,11 @@
         <v>0</v>
       </c>
       <c r="AB85" s="15">
-        <f t="shared" si="159"/>
+        <f t="shared" si="169"/>
         <v>0</v>
       </c>
       <c r="AC85" s="16">
-        <f t="shared" si="160"/>
+        <f t="shared" si="170"/>
         <v>0</v>
       </c>
     </row>
@@ -33537,7 +33537,7 @@
         <v>0.125</v>
       </c>
       <c r="I86" s="16">
-        <f t="shared" si="150"/>
+        <f t="shared" si="160"/>
         <v>0.125</v>
       </c>
       <c r="J86" s="11">
@@ -33548,11 +33548,11 @@
         <v>0.1</v>
       </c>
       <c r="L86" s="15">
-        <f t="shared" si="151"/>
+        <f t="shared" si="161"/>
         <v>0.1</v>
       </c>
       <c r="M86" s="16">
-        <f t="shared" si="152"/>
+        <f t="shared" si="162"/>
         <v>0.1</v>
       </c>
       <c r="N86" s="11">
@@ -33563,11 +33563,11 @@
         <v>0.05</v>
       </c>
       <c r="P86" s="15">
-        <f t="shared" si="153"/>
+        <f t="shared" si="163"/>
         <v>0.05</v>
       </c>
       <c r="Q86" s="16">
-        <f t="shared" si="154"/>
+        <f t="shared" si="164"/>
         <v>0.05</v>
       </c>
       <c r="R86" s="11">
@@ -33578,11 +33578,11 @@
         <v>1</v>
       </c>
       <c r="T86" s="15">
-        <f t="shared" si="155"/>
+        <f t="shared" si="165"/>
         <v>1</v>
       </c>
       <c r="U86" s="16">
-        <f t="shared" si="156"/>
+        <f t="shared" si="166"/>
         <v>1</v>
       </c>
       <c r="V86" s="11">
@@ -33593,11 +33593,11 @@
         <v>0.25</v>
       </c>
       <c r="X86" s="15">
-        <f t="shared" si="157"/>
+        <f t="shared" si="167"/>
         <v>0.25</v>
       </c>
       <c r="Y86" s="16">
-        <f t="shared" si="158"/>
+        <f t="shared" si="168"/>
         <v>0.25</v>
       </c>
       <c r="Z86" s="11">
@@ -33608,11 +33608,11 @@
         <v>0.375</v>
       </c>
       <c r="AB86" s="15">
-        <f t="shared" si="159"/>
+        <f t="shared" si="169"/>
         <v>0.375</v>
       </c>
       <c r="AC86" s="16">
-        <f t="shared" si="160"/>
+        <f t="shared" si="170"/>
         <v>0.375</v>
       </c>
     </row>
@@ -33641,7 +33641,7 @@
         <v>17.5</v>
       </c>
       <c r="I87" s="16">
-        <f t="shared" si="150"/>
+        <f t="shared" si="160"/>
         <v>17.5</v>
       </c>
       <c r="J87" s="11">
@@ -33652,11 +33652,11 @@
         <v>15</v>
       </c>
       <c r="L87" s="15">
-        <f t="shared" si="151"/>
+        <f t="shared" si="161"/>
         <v>15</v>
       </c>
       <c r="M87" s="16">
-        <f t="shared" si="152"/>
+        <f t="shared" si="162"/>
         <v>15</v>
       </c>
       <c r="N87" s="11">
@@ -33667,11 +33667,11 @@
         <v>17.5</v>
       </c>
       <c r="P87" s="15">
-        <f t="shared" si="153"/>
+        <f t="shared" si="163"/>
         <v>17.5</v>
       </c>
       <c r="Q87" s="16">
-        <f t="shared" si="154"/>
+        <f t="shared" si="164"/>
         <v>17.5</v>
       </c>
       <c r="R87" s="11">
@@ -33682,11 +33682,11 @@
         <v>25</v>
       </c>
       <c r="T87" s="15">
-        <f t="shared" si="155"/>
+        <f t="shared" si="165"/>
         <v>25</v>
       </c>
       <c r="U87" s="16">
-        <f t="shared" si="156"/>
+        <f t="shared" si="166"/>
         <v>25</v>
       </c>
       <c r="V87" s="11">
@@ -33697,11 +33697,11 @@
         <v>22.5</v>
       </c>
       <c r="X87" s="15">
-        <f t="shared" si="157"/>
+        <f t="shared" si="167"/>
         <v>22.5</v>
       </c>
       <c r="Y87" s="16">
-        <f t="shared" si="158"/>
+        <f t="shared" si="168"/>
         <v>22.5</v>
       </c>
       <c r="Z87" s="11">
@@ -33712,11 +33712,11 @@
         <v>17.5</v>
       </c>
       <c r="AB87" s="15">
-        <f t="shared" si="159"/>
+        <f t="shared" si="169"/>
         <v>17.5</v>
       </c>
       <c r="AC87" s="16">
-        <f t="shared" si="160"/>
+        <f t="shared" si="170"/>
         <v>17.5</v>
       </c>
     </row>
@@ -33742,7 +33742,7 @@
         <v>0</v>
       </c>
       <c r="I88" s="16">
-        <f t="shared" si="150"/>
+        <f t="shared" si="160"/>
         <v>0</v>
       </c>
       <c r="K88" s="12">
@@ -33750,11 +33750,11 @@
         <v>0</v>
       </c>
       <c r="L88" s="15">
-        <f t="shared" si="151"/>
+        <f t="shared" si="161"/>
         <v>0</v>
       </c>
       <c r="M88" s="16">
-        <f t="shared" si="152"/>
+        <f t="shared" si="162"/>
         <v>0</v>
       </c>
       <c r="O88" s="12">
@@ -33762,11 +33762,11 @@
         <v>0</v>
       </c>
       <c r="P88" s="15">
-        <f t="shared" si="153"/>
+        <f t="shared" si="163"/>
         <v>0</v>
       </c>
       <c r="Q88" s="16">
-        <f t="shared" si="154"/>
+        <f t="shared" si="164"/>
         <v>0</v>
       </c>
       <c r="S88" s="12">
@@ -33774,11 +33774,11 @@
         <v>0</v>
       </c>
       <c r="T88" s="15">
-        <f t="shared" si="155"/>
+        <f t="shared" si="165"/>
         <v>0</v>
       </c>
       <c r="U88" s="16">
-        <f t="shared" si="156"/>
+        <f t="shared" si="166"/>
         <v>0</v>
       </c>
       <c r="W88" s="12">
@@ -33786,11 +33786,11 @@
         <v>0</v>
       </c>
       <c r="X88" s="15">
-        <f t="shared" si="157"/>
+        <f t="shared" si="167"/>
         <v>0</v>
       </c>
       <c r="Y88" s="16">
-        <f t="shared" si="158"/>
+        <f t="shared" si="168"/>
         <v>0</v>
       </c>
       <c r="AA88" s="12">
@@ -33798,11 +33798,11 @@
         <v>0</v>
       </c>
       <c r="AB88" s="15">
-        <f t="shared" si="159"/>
+        <f t="shared" si="169"/>
         <v>0</v>
       </c>
       <c r="AC88" s="16">
-        <f t="shared" si="160"/>
+        <f t="shared" si="170"/>
         <v>0</v>
       </c>
     </row>
@@ -33826,67 +33826,67 @@
         <v>0</v>
       </c>
       <c r="I89" s="16">
-        <f t="shared" si="150"/>
+        <f t="shared" si="160"/>
         <v>0</v>
       </c>
       <c r="K89" s="12">
-        <f t="shared" ref="K89:K90" si="161">J89</f>
+        <f t="shared" ref="K89:K93" si="171">J89</f>
         <v>0</v>
       </c>
       <c r="L89" s="15">
-        <f t="shared" si="151"/>
+        <f t="shared" si="161"/>
         <v>0</v>
       </c>
       <c r="M89" s="16">
-        <f t="shared" si="152"/>
+        <f t="shared" si="162"/>
         <v>0</v>
       </c>
       <c r="O89" s="12">
-        <f t="shared" ref="O89:O90" si="162">N89</f>
+        <f t="shared" ref="O89:O93" si="172">N89</f>
         <v>0</v>
       </c>
       <c r="P89" s="15">
-        <f t="shared" si="153"/>
+        <f t="shared" si="163"/>
         <v>0</v>
       </c>
       <c r="Q89" s="16">
-        <f t="shared" si="154"/>
+        <f t="shared" si="164"/>
         <v>0</v>
       </c>
       <c r="S89" s="12">
-        <f t="shared" ref="S89:S90" si="163">R89</f>
+        <f t="shared" ref="S89:S93" si="173">R89</f>
         <v>0</v>
       </c>
       <c r="T89" s="15">
-        <f t="shared" si="155"/>
+        <f t="shared" si="165"/>
         <v>0</v>
       </c>
       <c r="U89" s="16">
-        <f t="shared" si="156"/>
+        <f t="shared" si="166"/>
         <v>0</v>
       </c>
       <c r="W89" s="12">
-        <f t="shared" ref="W89:W90" si="164">V89</f>
+        <f t="shared" ref="W89:W93" si="174">V89</f>
         <v>0</v>
       </c>
       <c r="X89" s="15">
-        <f t="shared" si="157"/>
+        <f t="shared" si="167"/>
         <v>0</v>
       </c>
       <c r="Y89" s="16">
-        <f t="shared" si="158"/>
+        <f t="shared" si="168"/>
         <v>0</v>
       </c>
       <c r="AA89" s="12">
-        <f t="shared" ref="AA89:AA90" si="165">Z89</f>
+        <f t="shared" ref="AA89:AA93" si="175">Z89</f>
         <v>0</v>
       </c>
       <c r="AB89" s="15">
-        <f t="shared" si="159"/>
+        <f t="shared" si="169"/>
         <v>0</v>
       </c>
       <c r="AC89" s="16">
-        <f t="shared" si="160"/>
+        <f t="shared" si="170"/>
         <v>0</v>
       </c>
     </row>
@@ -33910,67 +33910,67 @@
         <v>0</v>
       </c>
       <c r="I90" s="16">
-        <f t="shared" si="150"/>
+        <f t="shared" si="160"/>
         <v>0</v>
       </c>
       <c r="K90" s="12">
+        <f t="shared" si="171"/>
+        <v>0</v>
+      </c>
+      <c r="L90" s="15">
         <f t="shared" si="161"/>
         <v>0</v>
       </c>
-      <c r="L90" s="15">
-        <f t="shared" si="151"/>
-        <v>0</v>
-      </c>
       <c r="M90" s="16">
-        <f t="shared" si="152"/>
+        <f t="shared" si="162"/>
         <v>0</v>
       </c>
       <c r="O90" s="12">
-        <f t="shared" si="162"/>
+        <f t="shared" si="172"/>
         <v>0</v>
       </c>
       <c r="P90" s="15">
-        <f t="shared" si="153"/>
+        <f t="shared" si="163"/>
         <v>0</v>
       </c>
       <c r="Q90" s="16">
-        <f t="shared" si="154"/>
+        <f t="shared" si="164"/>
         <v>0</v>
       </c>
       <c r="S90" s="12">
-        <f t="shared" si="163"/>
+        <f t="shared" si="173"/>
         <v>0</v>
       </c>
       <c r="T90" s="15">
-        <f t="shared" si="155"/>
+        <f t="shared" si="165"/>
         <v>0</v>
       </c>
       <c r="U90" s="16">
-        <f t="shared" si="156"/>
+        <f t="shared" si="166"/>
         <v>0</v>
       </c>
       <c r="W90" s="12">
-        <f t="shared" si="164"/>
+        <f t="shared" si="174"/>
         <v>0</v>
       </c>
       <c r="X90" s="15">
-        <f t="shared" si="157"/>
+        <f t="shared" si="167"/>
         <v>0</v>
       </c>
       <c r="Y90" s="16">
-        <f t="shared" si="158"/>
+        <f t="shared" si="168"/>
         <v>0</v>
       </c>
       <c r="AA90" s="12">
-        <f t="shared" si="165"/>
+        <f t="shared" si="175"/>
         <v>0</v>
       </c>
       <c r="AB90" s="15">
-        <f t="shared" si="159"/>
+        <f t="shared" si="169"/>
         <v>0</v>
       </c>
       <c r="AC90" s="16">
-        <f t="shared" si="160"/>
+        <f t="shared" si="170"/>
         <v>0</v>
       </c>
     </row>
@@ -33996,7 +33996,7 @@
         <v>0</v>
       </c>
       <c r="I91" s="16">
-        <f t="shared" si="150"/>
+        <f t="shared" si="160"/>
         <v>0</v>
       </c>
       <c r="K91" s="12">
@@ -34004,11 +34004,11 @@
         <v>0</v>
       </c>
       <c r="L91" s="15">
-        <f t="shared" si="151"/>
+        <f t="shared" si="161"/>
         <v>0</v>
       </c>
       <c r="M91" s="16">
-        <f t="shared" si="152"/>
+        <f t="shared" si="162"/>
         <v>0</v>
       </c>
       <c r="O91" s="12">
@@ -34016,11 +34016,11 @@
         <v>0</v>
       </c>
       <c r="P91" s="15">
-        <f t="shared" si="153"/>
+        <f t="shared" si="163"/>
         <v>0</v>
       </c>
       <c r="Q91" s="16">
-        <f t="shared" si="154"/>
+        <f t="shared" si="164"/>
         <v>0</v>
       </c>
       <c r="R91" s="11">
@@ -34031,11 +34031,11 @@
         <v>4.5</v>
       </c>
       <c r="T91" s="15">
-        <f t="shared" si="155"/>
+        <f t="shared" si="165"/>
         <v>4.5</v>
       </c>
       <c r="U91" s="16">
-        <f t="shared" si="156"/>
+        <f t="shared" si="166"/>
         <v>4.5</v>
       </c>
       <c r="W91" s="12">
@@ -34043,11 +34043,11 @@
         <v>0</v>
       </c>
       <c r="X91" s="15">
-        <f t="shared" si="157"/>
+        <f t="shared" si="167"/>
         <v>0</v>
       </c>
       <c r="Y91" s="16">
-        <f t="shared" si="158"/>
+        <f t="shared" si="168"/>
         <v>0</v>
       </c>
       <c r="AA91" s="12">
@@ -34055,11 +34055,11 @@
         <v>0</v>
       </c>
       <c r="AB91" s="15">
-        <f t="shared" si="159"/>
+        <f t="shared" si="169"/>
         <v>0</v>
       </c>
       <c r="AC91" s="16">
-        <f t="shared" si="160"/>
+        <f t="shared" si="170"/>
         <v>0</v>
       </c>
     </row>
@@ -34083,70 +34083,70 @@
         <v>0</v>
       </c>
       <c r="I92" s="16">
-        <f t="shared" si="150"/>
+        <f t="shared" si="160"/>
         <v>0</v>
       </c>
       <c r="K92" s="12">
-        <f t="shared" ref="K92:K93" si="166">J92</f>
+        <f t="shared" ref="K92:K93" si="176">J92</f>
         <v>0</v>
       </c>
       <c r="L92" s="15">
-        <f t="shared" si="151"/>
+        <f t="shared" si="161"/>
         <v>0</v>
       </c>
       <c r="M92" s="16">
-        <f t="shared" si="152"/>
+        <f t="shared" si="162"/>
         <v>0</v>
       </c>
       <c r="O92" s="12">
-        <f t="shared" ref="O92:O93" si="167">N92</f>
+        <f t="shared" ref="O92:O93" si="177">N92</f>
         <v>0</v>
       </c>
       <c r="P92" s="15">
-        <f t="shared" si="153"/>
+        <f t="shared" si="163"/>
         <v>0</v>
       </c>
       <c r="Q92" s="16">
-        <f t="shared" si="154"/>
+        <f t="shared" si="164"/>
         <v>0</v>
       </c>
       <c r="R92" s="11">
         <v>1</v>
       </c>
       <c r="S92" s="12">
-        <f t="shared" ref="S92:S93" si="168">R92</f>
+        <f t="shared" ref="S92:S93" si="178">R92</f>
         <v>1</v>
       </c>
       <c r="T92" s="15">
-        <f t="shared" si="155"/>
+        <f t="shared" si="165"/>
         <v>1</v>
       </c>
       <c r="U92" s="16">
-        <f t="shared" si="156"/>
+        <f t="shared" si="166"/>
         <v>1</v>
       </c>
       <c r="W92" s="12">
-        <f t="shared" ref="W92:W93" si="169">V92</f>
+        <f t="shared" ref="W92:W93" si="179">V92</f>
         <v>0</v>
       </c>
       <c r="X92" s="15">
-        <f t="shared" si="157"/>
+        <f t="shared" si="167"/>
         <v>0</v>
       </c>
       <c r="Y92" s="16">
-        <f t="shared" si="158"/>
+        <f t="shared" si="168"/>
         <v>0</v>
       </c>
       <c r="AA92" s="12">
-        <f t="shared" ref="AA92:AA93" si="170">Z92</f>
+        <f t="shared" ref="AA92:AA93" si="180">Z92</f>
         <v>0</v>
       </c>
       <c r="AB92" s="15">
-        <f t="shared" si="159"/>
+        <f t="shared" si="169"/>
         <v>0</v>
       </c>
       <c r="AC92" s="16">
-        <f t="shared" si="160"/>
+        <f t="shared" si="170"/>
         <v>0</v>
       </c>
     </row>
@@ -34170,70 +34170,70 @@
         <v>0</v>
       </c>
       <c r="I93" s="16">
-        <f t="shared" si="150"/>
+        <f t="shared" si="160"/>
         <v>0</v>
       </c>
       <c r="K93" s="12">
-        <f t="shared" si="166"/>
+        <f t="shared" si="176"/>
         <v>0</v>
       </c>
       <c r="L93" s="15">
-        <f t="shared" si="151"/>
+        <f t="shared" si="161"/>
         <v>0</v>
       </c>
       <c r="M93" s="16">
-        <f t="shared" si="152"/>
+        <f t="shared" si="162"/>
         <v>0</v>
       </c>
       <c r="O93" s="12">
-        <f t="shared" si="167"/>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="P93" s="15">
-        <f t="shared" si="153"/>
+        <f t="shared" si="163"/>
         <v>0</v>
       </c>
       <c r="Q93" s="16">
-        <f t="shared" si="154"/>
+        <f t="shared" si="164"/>
         <v>0</v>
       </c>
       <c r="R93" s="11">
         <v>5</v>
       </c>
       <c r="S93" s="12">
+        <f t="shared" si="178"/>
+        <v>5</v>
+      </c>
+      <c r="T93" s="15">
+        <f t="shared" si="165"/>
+        <v>5</v>
+      </c>
+      <c r="U93" s="16">
+        <f t="shared" si="166"/>
+        <v>5</v>
+      </c>
+      <c r="W93" s="12">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="X93" s="15">
+        <f t="shared" si="167"/>
+        <v>0</v>
+      </c>
+      <c r="Y93" s="16">
         <f t="shared" si="168"/>
-        <v>5</v>
-      </c>
-      <c r="T93" s="15">
-        <f t="shared" si="155"/>
-        <v>5</v>
-      </c>
-      <c r="U93" s="16">
-        <f t="shared" si="156"/>
-        <v>5</v>
-      </c>
-      <c r="W93" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA93" s="12">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="AB93" s="15">
         <f t="shared" si="169"/>
         <v>0</v>
       </c>
-      <c r="X93" s="15">
-        <f t="shared" si="157"/>
-        <v>0</v>
-      </c>
-      <c r="Y93" s="16">
-        <f t="shared" si="158"/>
-        <v>0</v>
-      </c>
-      <c r="AA93" s="12">
+      <c r="AC93" s="16">
         <f t="shared" si="170"/>
-        <v>0</v>
-      </c>
-      <c r="AB93" s="15">
-        <f t="shared" si="159"/>
-        <v>0</v>
-      </c>
-      <c r="AC93" s="16">
-        <f t="shared" si="160"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>